<commit_message>
redefined leh11 --> leh33, leh33 --> leh21, leh44 --> leh51
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
+++ b/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA22BD10-4548-C842-BC65-1A1F35E6B914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D38A5F-0DE5-6643-9F5F-8D69A73B5349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="singlish_NUS_SMS" sheetId="1" r:id="rId1"/>
@@ -29220,8 +29220,8 @@
   <dimension ref="A1:H2245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A519" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E521" sqref="E521"/>
+      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A481" sqref="A481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
LABEL [YZ] [NUS SMS dataset] redefined leh11 --> leh33, leh33 --> leh21, leh44 --> leh51
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
+++ b/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D38A5F-0DE5-6643-9F5F-8D69A73B5349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51146EF9-DE8A-5E44-BD71-00C323553054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27616,9 +27616,6 @@
     <t>["lor33"]</t>
   </si>
   <si>
-    <t>["lor33", "leh11"]</t>
-  </si>
-  <si>
     <t>["lah21", "lor33"]</t>
   </si>
   <si>
@@ -27628,9 +27625,6 @@
     <t>["lah21","lah21"]</t>
   </si>
   <si>
-    <t>["lah24", "leh11"]</t>
-  </si>
-  <si>
     <t>["lah24"]</t>
   </si>
   <si>
@@ -27640,40 +27634,16 @@
     <t>["lah51"]</t>
   </si>
   <si>
-    <t>["leh11", "lah21"]</t>
-  </si>
-  <si>
-    <t>["leh11", "lah51", "lor33"]</t>
-  </si>
-  <si>
-    <t>["leh11", "leh33"]</t>
-  </si>
-  <si>
-    <t>["leh11", "lor33"]</t>
-  </si>
-  <si>
-    <t>["leh11"]</t>
-  </si>
-  <si>
     <t>["leh33", "lah21"]</t>
   </si>
   <si>
-    <t>["leh33", "leh11"]</t>
-  </si>
-  <si>
     <t>["leh33", "lor33"]</t>
   </si>
   <si>
     <t>["leh33"]</t>
   </si>
   <si>
-    <t>["leh44"]</t>
-  </si>
-  <si>
     <t>["lor33", "leh33"]</t>
-  </si>
-  <si>
-    <t>["lor33", "leh11", "lah51"]</t>
   </si>
   <si>
     <t>["lor33", "lah21"]</t>
@@ -27836,9 +27806,6 @@
 B: Obviously I didn't lah, maybe telegram spoil</t>
   </si>
   <si>
-    <t>["leh33", "lah51"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: I am the master of multitasking
 B: u sure you can beat me?
@@ -28008,9 +27975,6 @@
     <t>added more relevant singlish particles</t>
   </si>
   <si>
-    <t>["lah21", "leh11", "lah51", "lor33"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey, are you coming to the concert tonight?
 B: I don't know, it's so last minute and I don't have a ticket.
@@ -28040,16 +28004,10 @@
     <t>restrict to 5 utterances</t>
   </si>
   <si>
-    <t>["lah21","leh11", "lah24"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Why you never tell us earlier, we could have went to find you
 B: Aiya, never mind lah. Now it's already so late.
 C: Tomorrow leh, do you have plans?</t>
-  </si>
-  <si>
-    <t>["lah21", "leh11"]</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -28081,9 +28039,6 @@
 B: No lah, our relationship is not even confirmed, will see how it goes lah</t>
   </si>
   <si>
-    <t>["leh11", "lah21", "lah24"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey, have you decided on which salon to go get a haircut?
 B: I'm thinking of going to salon4hair, but I'm not sure how much it is
@@ -28208,16 +28163,10 @@
 B: You see me then alight lor</t>
   </si>
   <si>
-    <t>["leh33","lah21"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey guys, are you free tonight?
 B: Yeah, why leh?
 A: I was thinking of watching the sneak preview of the new movie lor. Anyone interested?</t>
-  </si>
-  <si>
-    <t>["leh11","lor33"]</t>
   </si>
   <si>
     <t>removed last utterance as it was irrelevant. Added new utternace to make the convo lively.</t>
@@ -28233,9 +28182,6 @@
     <t>added "lah" to show tone</t>
   </si>
   <si>
-    <t>["leh11","lah21","lah21"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey, how was your birthday?
 B: It was okay lah. I didn't do much leh.
@@ -28255,9 +28201,6 @@
 added singlish particle to improve flow</t>
   </si>
   <si>
-    <t>["lor33","leh11"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hi guys, I'm heading to the grocery store. Anything you want me to get?
 B: No need lah
@@ -28268,9 +28211,6 @@
 added singlish particle </t>
   </si>
   <si>
-    <t>["lah21","leh11"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Oh, the event is on Wednesday, isn't it? 
 B: Yes, it is. Are you planning to attend too? 
@@ -28295,9 +28235,6 @@
 A: Hey, I saw you on Monday outside the mall, why were you in such a hurry that day?
 B: Er Monday, no particular reason leh, I probably just walk fast
 A: Okay lah you long legs lor</t>
-  </si>
-  <si>
-    <t>["leh11","lah21", "lor33"]</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -28368,9 +28305,6 @@
 B: Why leh? You've been practicing for weeks.
 A: Yeah, but I might trip and not know what to say lor
 B: Don't worry, you'll do great. Just trust yourself lah.</t>
-  </si>
-  <si>
-    <t>["leh11", "lor33", "lah21"]</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -28411,9 +28345,6 @@
     <t>shorten utterances and make it more relevant</t>
   </si>
   <si>
-    <t>["lah21", "leh11", "leh33"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">it should be "then meet what time ah" but we are not interested in ah particle </t>
   </si>
   <si>
@@ -28445,9 +28376,6 @@
   </si>
   <si>
     <t>reorder the convo and make the particles the focus, introduce new lah particle in the convo</t>
-  </si>
-  <si>
-    <t>["leh11", "lah24"]</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -28518,9 +28446,6 @@
     <t>reorder convo</t>
   </si>
   <si>
-    <t>["lah51", "leh11"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey, did you manage to enrol for the course?
 B: No leh, it's fully enrolled already
@@ -28746,9 +28671,6 @@
 B: Well, we've been here for five hours already and we haven't made much progress. Maybe we should just call it a night and continue tomorrow.</t>
   </si>
   <si>
-    <t>["lor33", "leh11"}</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: meet you guys again tomorrow?
 B: Don't want lah, I have been seeing you too much recently</t>
@@ -28812,6 +28734,84 @@
 B: Oh, mostly clothes and accessories leh
 A: don't you have a lot already in the cupboard
 B: I mean girls love shopping and we can’t help it lor</t>
+  </si>
+  <si>
+    <t>["leh51"]</t>
+  </si>
+  <si>
+    <t>["leh21"]</t>
+  </si>
+  <si>
+    <t>["lor33", "leh21"]</t>
+  </si>
+  <si>
+    <t>["leh21", "lor33"]</t>
+  </si>
+  <si>
+    <t>["leh21", "lah21"]</t>
+  </si>
+  <si>
+    <t>["leh21", "lah51"]</t>
+  </si>
+  <si>
+    <t>["leh21","lah21"]</t>
+  </si>
+  <si>
+    <t>["leh33", "leh21"]</t>
+  </si>
+  <si>
+    <t>["leh21", "leh33"]</t>
+  </si>
+  <si>
+    <t>["leh33", "lah51", "lor33"]</t>
+  </si>
+  <si>
+    <t>["lor33", "leh33", "lah51"]</t>
+  </si>
+  <si>
+    <t>["lah24", "leh33"]</t>
+  </si>
+  <si>
+    <t>["lah21", "leh33", "lah51", "lor33"]</t>
+  </si>
+  <si>
+    <t>["lah21","leh33", "lah24"]</t>
+  </si>
+  <si>
+    <t>["lah21", "leh33"]</t>
+  </si>
+  <si>
+    <t>["leh33", "lah21", "lah24"]</t>
+  </si>
+  <si>
+    <t>["leh33","lah21", "lor33"]</t>
+  </si>
+  <si>
+    <t>["leh33","lor33"]</t>
+  </si>
+  <si>
+    <t>["leh33","lah21","lah21"]</t>
+  </si>
+  <si>
+    <t>["lor33","leh33"]</t>
+  </si>
+  <si>
+    <t>["lah21","leh33"]</t>
+  </si>
+  <si>
+    <t>["leh33", "lor33", "lah21"]</t>
+  </si>
+  <si>
+    <t>["lah21", "leh33", "leh21"]</t>
+  </si>
+  <si>
+    <t>["leh33", "lah24"]</t>
+  </si>
+  <si>
+    <t>["lah51", "leh33"]</t>
+  </si>
+  <si>
+    <t>["lor33", "leh33"}</t>
   </si>
 </sst>
 </file>
@@ -29219,9 +29219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A481" sqref="A481"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29369,7 +29369,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>4579</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="112" x14ac:dyDescent="0.2">
@@ -29415,7 +29415,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="96" x14ac:dyDescent="0.2">
@@ -29478,7 +29478,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="112" x14ac:dyDescent="0.2">
@@ -29541,7 +29541,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="128" x14ac:dyDescent="0.2">
@@ -29564,7 +29564,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.2">
@@ -29587,7 +29587,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -29656,7 +29656,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -29679,7 +29679,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -29702,7 +29702,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30101,7 +30101,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>4596</v>
+        <v>4804</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -30146,7 +30146,7 @@
         <v>2</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -30169,7 +30169,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="176" x14ac:dyDescent="0.2">
@@ -30236,7 +30236,7 @@
         <v>2</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>4589</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30303,7 +30303,7 @@
         <v>2</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>4593</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30359,7 +30359,7 @@
         <v>2</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>4597</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30382,7 +30382,7 @@
         <v>2</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -30460,7 +30460,7 @@
         <v>2</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>4594</v>
+        <v>4807</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30483,7 +30483,7 @@
         <v>3</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>4588</v>
+        <v>4813</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30583,7 +30583,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30650,7 +30650,7 @@
         <v>2</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>4594</v>
+        <v>4807</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -30717,7 +30717,7 @@
         <v>1</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30751,7 +30751,7 @@
         <v>2</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>4592</v>
+        <v>4808</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30829,7 +30829,7 @@
         <v>1</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -30885,7 +30885,7 @@
         <v>1</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -31018,7 +31018,7 @@
         <v>2</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>4579</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -31129,7 +31129,7 @@
         <v>2</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>4579</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -31163,7 +31163,7 @@
         <v>3</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>4598</v>
+        <v>4814</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -31439,7 +31439,7 @@
         <v>2</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>4592</v>
+        <v>4808</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -31539,7 +31539,7 @@
         <v>1</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -31562,7 +31562,7 @@
         <v>1</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="166" spans="1:7" s="5" customFormat="1" ht="128" x14ac:dyDescent="0.2">
@@ -31585,7 +31585,7 @@
         <v>2</v>
       </c>
       <c r="G166" s="5" t="s">
-        <v>4585</v>
+        <v>4583</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -31620,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -31643,7 +31643,7 @@
         <v>1</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -31677,7 +31677,7 @@
         <v>1</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -31700,7 +31700,7 @@
         <v>2</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>4583</v>
+        <v>4815</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -31723,7 +31723,7 @@
         <v>1</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -31746,7 +31746,7 @@
         <v>1</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -31769,7 +31769,7 @@
         <v>1</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -31803,7 +31803,7 @@
         <v>1</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -31826,7 +31826,7 @@
         <v>2</v>
       </c>
       <c r="G178" s="6" t="s">
-        <v>4582</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -31849,7 +31849,7 @@
         <v>2</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>4599</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -31872,7 +31872,7 @@
         <v>1</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -31895,7 +31895,7 @@
         <v>1</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -31962,7 +31962,7 @@
         <v>2</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>4592</v>
+        <v>4808</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -31985,7 +31985,7 @@
         <v>1</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32008,7 +32008,7 @@
         <v>1</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32031,7 +32031,7 @@
         <v>1</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32098,7 +32098,7 @@
         <v>1</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32121,7 +32121,7 @@
         <v>2</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32161,7 +32161,7 @@
         <v>2</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -32184,7 +32184,7 @@
         <v>1</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32218,7 +32218,7 @@
         <v>1</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32241,7 +32241,7 @@
         <v>1</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32264,7 +32264,7 @@
         <v>1</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32287,7 +32287,7 @@
         <v>1</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32310,7 +32310,7 @@
         <v>1</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32344,7 +32344,7 @@
         <v>1</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="207" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32367,7 +32367,7 @@
         <v>2</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>4579</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32390,7 +32390,7 @@
         <v>1</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="209" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32413,7 +32413,7 @@
         <v>2</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32436,7 +32436,7 @@
         <v>2</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32459,7 +32459,7 @@
         <v>1</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="212" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32493,7 +32493,7 @@
         <v>1</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32504,7 +32504,7 @@
         <v>2414</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>4600</v>
+        <v>4590</v>
       </c>
       <c r="D214" t="b">
         <v>1</v>
@@ -32527,7 +32527,7 @@
         <v>2415</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>4601</v>
+        <v>4591</v>
       </c>
       <c r="D215" t="b">
         <v>1</v>
@@ -32539,7 +32539,7 @@
         <v>1</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="216" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32550,7 +32550,7 @@
         <v>2416</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>4602</v>
+        <v>4592</v>
       </c>
       <c r="D216" t="b">
         <v>1</v>
@@ -32573,7 +32573,7 @@
         <v>2417</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>4603</v>
+        <v>4593</v>
       </c>
       <c r="D217" t="b">
         <v>1</v>
@@ -32585,7 +32585,7 @@
         <v>1</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32596,7 +32596,7 @@
         <v>2418</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>4604</v>
+        <v>4594</v>
       </c>
       <c r="D218" t="b">
         <v>1</v>
@@ -32608,7 +32608,7 @@
         <v>1</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -32619,7 +32619,7 @@
         <v>2419</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>4605</v>
+        <v>4595</v>
       </c>
       <c r="D219" t="b">
         <v>1</v>
@@ -32631,7 +32631,7 @@
         <v>1</v>
       </c>
       <c r="G219" s="6" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="176" x14ac:dyDescent="0.2">
@@ -32642,7 +32642,7 @@
         <v>2420</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>4606</v>
+        <v>4596</v>
       </c>
       <c r="D220" t="b">
         <v>1</v>
@@ -32654,7 +32654,7 @@
         <v>1</v>
       </c>
       <c r="G220" s="6" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32665,19 +32665,19 @@
         <v>2421</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>4607</v>
+        <v>4597</v>
       </c>
       <c r="D221" t="b">
         <v>1</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>4608</v>
+        <v>4598</v>
       </c>
       <c r="F221">
         <v>1</v>
       </c>
       <c r="G221" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="222" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32688,13 +32688,13 @@
         <v>2422</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>4609</v>
+        <v>4599</v>
       </c>
       <c r="D222" t="b">
         <v>1</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>4610</v>
+        <v>4600</v>
       </c>
       <c r="F222">
         <v>1</v>
@@ -32744,7 +32744,7 @@
         <v>2426</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>4611</v>
+        <v>4601</v>
       </c>
       <c r="D226" t="b">
         <v>1</v>
@@ -32756,7 +32756,7 @@
         <v>1</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -32822,7 +32822,7 @@
         <v>2432</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>4612</v>
+        <v>4602</v>
       </c>
       <c r="D232" t="b">
         <v>1</v>
@@ -32834,7 +32834,7 @@
         <v>1</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32845,7 +32845,7 @@
         <v>2433</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>4613</v>
+        <v>4603</v>
       </c>
       <c r="D233" t="b">
         <v>1</v>
@@ -32857,7 +32857,7 @@
         <v>1</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="234" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32879,19 +32879,19 @@
         <v>2435</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>4615</v>
+        <v>4605</v>
       </c>
       <c r="D235" t="b">
         <v>1</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>4614</v>
+        <v>4604</v>
       </c>
       <c r="F235">
         <v>2</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="236" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32913,7 +32913,7 @@
         <v>2437</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>4616</v>
+        <v>4606</v>
       </c>
       <c r="D237" t="b">
         <v>1</v>
@@ -32925,7 +32925,7 @@
         <v>1</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="238" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -32936,7 +32936,7 @@
         <v>2438</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>4617</v>
+        <v>4607</v>
       </c>
       <c r="D238" t="b">
         <v>1</v>
@@ -33025,19 +33025,19 @@
         <v>2445</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>4618</v>
+        <v>4608</v>
       </c>
       <c r="D245" t="b">
         <v>1</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>4619</v>
+        <v>4609</v>
       </c>
       <c r="F245">
         <v>2</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>4582</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33048,19 +33048,19 @@
         <v>2446</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>4620</v>
+        <v>4610</v>
       </c>
       <c r="D246" t="b">
         <v>1</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>4621</v>
+        <v>4611</v>
       </c>
       <c r="F246">
         <v>1</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="247" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33071,7 +33071,7 @@
         <v>2447</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>4622</v>
+        <v>4612</v>
       </c>
       <c r="D247" t="b">
         <v>1</v>
@@ -33083,7 +33083,7 @@
         <v>1</v>
       </c>
       <c r="G247" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="248" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33105,19 +33105,19 @@
         <v>2449</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>4623</v>
+        <v>4613</v>
       </c>
       <c r="D249" t="b">
         <v>1</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>4624</v>
+        <v>4614</v>
       </c>
       <c r="F249">
         <v>1</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="250" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33128,19 +33128,19 @@
         <v>2450</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>4626</v>
+        <v>4616</v>
       </c>
       <c r="D250" t="b">
         <v>1</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>4625</v>
+        <v>4615</v>
       </c>
       <c r="F250">
         <v>2</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="251" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33151,7 +33151,7 @@
         <v>2451</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>4627</v>
+        <v>4617</v>
       </c>
       <c r="D251" t="b">
         <v>1</v>
@@ -33163,7 +33163,7 @@
         <v>2</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>4628</v>
+        <v>4809</v>
       </c>
     </row>
     <row r="252" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33174,19 +33174,19 @@
         <v>2452</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>4629</v>
+        <v>4618</v>
       </c>
       <c r="D252" t="b">
         <v>1</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>4610</v>
+        <v>4600</v>
       </c>
       <c r="F252">
         <v>2</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>4592</v>
+        <v>4808</v>
       </c>
     </row>
     <row r="253" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33197,19 +33197,19 @@
         <v>2453</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>4630</v>
+        <v>4619</v>
       </c>
       <c r="D253" t="b">
         <v>1</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>4631</v>
+        <v>4620</v>
       </c>
       <c r="F253">
         <v>1</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="254" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33220,19 +33220,19 @@
         <v>2454</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>4632</v>
+        <v>4621</v>
       </c>
       <c r="D254" t="b">
         <v>1</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>4635</v>
+        <v>4624</v>
       </c>
       <c r="F254">
         <v>1</v>
       </c>
       <c r="G254" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="255" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33243,19 +33243,19 @@
         <v>2455</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>4633</v>
+        <v>4622</v>
       </c>
       <c r="D255" t="b">
         <v>1</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>4634</v>
+        <v>4623</v>
       </c>
       <c r="F255">
         <v>1</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="256" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33266,19 +33266,19 @@
         <v>2456</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>4637</v>
+        <v>4626</v>
       </c>
       <c r="D256" t="b">
         <v>1</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>4636</v>
+        <v>4625</v>
       </c>
       <c r="F256">
         <v>1</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="257" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -33289,19 +33289,19 @@
         <v>2457</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>4638</v>
+        <v>4627</v>
       </c>
       <c r="D257" t="b">
         <v>1</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>4639</v>
+        <v>4628</v>
       </c>
       <c r="F257">
         <v>1</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="258" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33312,7 +33312,7 @@
         <v>2458</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>4640</v>
+        <v>4629</v>
       </c>
       <c r="D258" t="b">
         <v>1</v>
@@ -33324,7 +33324,7 @@
         <v>1</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="259" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -33335,7 +33335,7 @@
         <v>2459</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>4641</v>
+        <v>4630</v>
       </c>
       <c r="D259" t="b">
         <v>1</v>
@@ -33347,7 +33347,7 @@
         <v>1</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="260" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33358,19 +33358,19 @@
         <v>2460</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>4642</v>
+        <v>4631</v>
       </c>
       <c r="D260" t="b">
         <v>1</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>4643</v>
+        <v>4632</v>
       </c>
       <c r="F260">
         <v>2</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>4583</v>
+        <v>4815</v>
       </c>
     </row>
     <row r="261" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33381,19 +33381,19 @@
         <v>2461</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>4644</v>
+        <v>4633</v>
       </c>
       <c r="D261" t="b">
         <v>1</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>4645</v>
+        <v>4634</v>
       </c>
       <c r="F261">
         <v>1</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="262" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33404,19 +33404,19 @@
         <v>2462</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>4646</v>
+        <v>4635</v>
       </c>
       <c r="D262" t="b">
         <v>1</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>4647</v>
+        <v>4636</v>
       </c>
       <c r="F262">
         <v>2</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>4648</v>
+        <v>4637</v>
       </c>
     </row>
     <row r="263" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33427,19 +33427,19 @@
         <v>2463</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>4649</v>
+        <v>4638</v>
       </c>
       <c r="D263" t="b">
         <v>1</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F263">
         <v>1</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="264" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33450,19 +33450,19 @@
         <v>2464</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>4651</v>
+        <v>4640</v>
       </c>
       <c r="D264" t="b">
         <v>1</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>4652</v>
+        <v>4641</v>
       </c>
       <c r="F264">
         <v>2</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>4628</v>
+        <v>4809</v>
       </c>
     </row>
     <row r="265" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33473,7 +33473,7 @@
         <v>2465</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>4653</v>
+        <v>4642</v>
       </c>
       <c r="D265" t="b">
         <v>1</v>
@@ -33502,13 +33502,13 @@
         <v>1</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>4654</v>
+        <v>4643</v>
       </c>
       <c r="F266">
         <v>1</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="267" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33519,19 +33519,19 @@
         <v>2467</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>4655</v>
+        <v>4644</v>
       </c>
       <c r="D267" t="b">
         <v>1</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>4656</v>
+        <v>4645</v>
       </c>
       <c r="F267">
         <v>2</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>4597</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="268" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -33542,13 +33542,13 @@
         <v>2468</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>4657</v>
+        <v>4646</v>
       </c>
       <c r="D268" t="b">
         <v>1</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>4658</v>
+        <v>4647</v>
       </c>
       <c r="F268">
         <v>1</v>
@@ -33565,19 +33565,19 @@
         <v>2469</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>4659</v>
+        <v>4648</v>
       </c>
       <c r="D269" t="b">
         <v>1</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>4660</v>
+        <v>4649</v>
       </c>
       <c r="F269">
         <v>2</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>4593</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="270" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -33588,7 +33588,7 @@
         <v>2470</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>4661</v>
+        <v>4650</v>
       </c>
       <c r="D270" t="b">
         <v>1</v>
@@ -33600,7 +33600,7 @@
         <v>2</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>4579</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="271" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33611,19 +33611,19 @@
         <v>2471</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>4662</v>
+        <v>4651</v>
       </c>
       <c r="D271" t="b">
         <v>1</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>4663</v>
+        <v>4652</v>
       </c>
       <c r="F271">
         <v>4</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>4664</v>
+        <v>4816</v>
       </c>
     </row>
     <row r="272" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33678,19 +33678,19 @@
         <v>2476</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>4665</v>
+        <v>4653</v>
       </c>
       <c r="D276" t="b">
         <v>1</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>4666</v>
+        <v>4654</v>
       </c>
       <c r="F276">
         <v>1</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="277" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33701,7 +33701,7 @@
         <v>2477</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>4667</v>
+        <v>4655</v>
       </c>
       <c r="D277" t="b">
         <v>1</v>
@@ -33713,7 +33713,7 @@
         <v>1</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="278" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33724,19 +33724,19 @@
         <v>2478</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>4668</v>
+        <v>4656</v>
       </c>
       <c r="D278" t="b">
         <v>1</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>4669</v>
+        <v>4657</v>
       </c>
       <c r="F278">
         <v>3</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>4670</v>
+        <v>4817</v>
       </c>
     </row>
     <row r="279" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -33802,7 +33802,7 @@
         <v>2484</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>4671</v>
+        <v>4658</v>
       </c>
       <c r="D284" t="b">
         <v>1</v>
@@ -33814,7 +33814,7 @@
         <v>2</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>4672</v>
+        <v>4818</v>
       </c>
     </row>
     <row r="285" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33825,13 +33825,13 @@
         <v>2485</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>4673</v>
+        <v>4659</v>
       </c>
       <c r="D285" t="b">
         <v>1</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>4674</v>
+        <v>4660</v>
       </c>
       <c r="F285">
         <v>1</v>
@@ -33859,19 +33859,19 @@
         <v>2487</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>4675</v>
+        <v>4661</v>
       </c>
       <c r="D287" t="b">
         <v>1</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>4676</v>
+        <v>4662</v>
       </c>
       <c r="F287">
         <v>2</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="288" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -33882,19 +33882,19 @@
         <v>2488</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>4678</v>
+        <v>4664</v>
       </c>
       <c r="D288" t="b">
         <v>1</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>4677</v>
+        <v>4663</v>
       </c>
       <c r="F288">
         <v>3</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>4679</v>
+        <v>4819</v>
       </c>
     </row>
     <row r="289" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33905,19 +33905,19 @@
         <v>2489</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>4680</v>
+        <v>4665</v>
       </c>
       <c r="D289" t="b">
         <v>1</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>4681</v>
+        <v>4666</v>
       </c>
       <c r="F289">
         <v>1</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="290" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33928,19 +33928,19 @@
         <v>2490</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>4682</v>
+        <v>4667</v>
       </c>
       <c r="D290" t="b">
         <v>1</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>4683</v>
+        <v>4668</v>
       </c>
       <c r="F290">
         <v>1</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="291" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34017,19 +34017,19 @@
         <v>2497</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>4684</v>
+        <v>4669</v>
       </c>
       <c r="D297" t="b">
         <v>1</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>4685</v>
+        <v>4670</v>
       </c>
       <c r="F297">
         <v>2</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="298" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34073,19 +34073,19 @@
         <v>2501</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>4686</v>
+        <v>4671</v>
       </c>
       <c r="D301" t="b">
         <v>1</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="F301">
         <v>1</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="302" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -34096,19 +34096,19 @@
         <v>2502</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>4688</v>
+        <v>4673</v>
       </c>
       <c r="D302" t="b">
         <v>1</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>4689</v>
+        <v>4674</v>
       </c>
       <c r="F302">
         <v>2</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="303" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -34130,19 +34130,19 @@
         <v>2504</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>4690</v>
+        <v>4675</v>
       </c>
       <c r="D304" t="b">
         <v>1</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>4691</v>
+        <v>4676</v>
       </c>
       <c r="F304">
         <v>2</v>
       </c>
       <c r="G304" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="305" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34186,19 +34186,19 @@
         <v>2508</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>4692</v>
+        <v>4677</v>
       </c>
       <c r="D308" t="b">
         <v>1</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>4693</v>
+        <v>4678</v>
       </c>
       <c r="F308">
         <v>2</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>4672</v>
+        <v>4818</v>
       </c>
     </row>
     <row r="309" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34231,19 +34231,19 @@
         <v>2511</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>4694</v>
+        <v>4679</v>
       </c>
       <c r="D311" t="b">
         <v>1</v>
       </c>
       <c r="E311" s="1" t="s">
-        <v>4695</v>
+        <v>4680</v>
       </c>
       <c r="F311">
         <v>2</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>4583</v>
+        <v>4815</v>
       </c>
     </row>
     <row r="312" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -34265,7 +34265,7 @@
         <v>2513</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>4696</v>
+        <v>4681</v>
       </c>
       <c r="D313" t="b">
         <v>1</v>
@@ -34277,7 +34277,7 @@
         <v>1</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="314" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34354,19 +34354,19 @@
         <v>2520</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>4697</v>
+        <v>4682</v>
       </c>
       <c r="D320" t="b">
         <v>1</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>4698</v>
+        <v>4683</v>
       </c>
       <c r="F320">
         <v>2</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="321" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -34465,19 +34465,19 @@
         <v>2529</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>4699</v>
+        <v>4684</v>
       </c>
       <c r="D329" t="b">
         <v>1</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F329">
         <v>1</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="330" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34532,19 +34532,19 @@
         <v>2534</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>4700</v>
+        <v>4685</v>
       </c>
       <c r="D334" t="b">
         <v>1</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>4701</v>
+        <v>4686</v>
       </c>
       <c r="F334">
         <v>2</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="335" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34566,19 +34566,19 @@
         <v>2536</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>4702</v>
+        <v>4687</v>
       </c>
       <c r="D336" t="b">
         <v>1</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F336">
         <v>1</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="337" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -34611,19 +34611,19 @@
         <v>2539</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>4703</v>
+        <v>4688</v>
       </c>
       <c r="D339" t="b">
         <v>1</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>4704</v>
+        <v>4689</v>
       </c>
       <c r="F339">
         <v>2</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="340" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34656,13 +34656,13 @@
         <v>2542</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>4705</v>
+        <v>4690</v>
       </c>
       <c r="D342" t="b">
         <v>1</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F342">
         <v>1</v>
@@ -34756,19 +34756,19 @@
         <v>2550</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>4726</v>
+        <v>4706</v>
       </c>
       <c r="D350" t="b">
         <v>1</v>
       </c>
       <c r="E350" s="1" t="s">
-        <v>4663</v>
+        <v>4652</v>
       </c>
       <c r="F350">
         <v>3</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>4727</v>
+        <v>4820</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -34779,7 +34779,7 @@
         <v>2551</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>4707</v>
+        <v>4691</v>
       </c>
       <c r="D351" t="b">
         <v>1</v>
@@ -34791,7 +34791,7 @@
         <v>2</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>4708</v>
+        <v>4821</v>
       </c>
     </row>
     <row r="352" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34802,19 +34802,19 @@
         <v>2552</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>4728</v>
+        <v>4707</v>
       </c>
       <c r="D352" t="b">
         <v>1</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>4709</v>
+        <v>4692</v>
       </c>
       <c r="F352">
         <v>2</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>4706</v>
+        <v>4810</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -34825,19 +34825,19 @@
         <v>2553</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>4729</v>
+        <v>4708</v>
       </c>
       <c r="D353" t="b">
         <v>1</v>
       </c>
       <c r="E353" s="1" t="s">
-        <v>4730</v>
+        <v>4709</v>
       </c>
       <c r="F353">
         <v>2</v>
       </c>
       <c r="G353" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="354" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34848,19 +34848,19 @@
         <v>2554</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>4710</v>
+        <v>4693</v>
       </c>
       <c r="D354" t="b">
         <v>1</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>4711</v>
+        <v>4694</v>
       </c>
       <c r="F354">
         <v>3</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>4712</v>
+        <v>4822</v>
       </c>
     </row>
     <row r="355" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34871,13 +34871,13 @@
         <v>2555</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>4713</v>
+        <v>4695</v>
       </c>
       <c r="D355" t="b">
         <v>0</v>
       </c>
       <c r="E355" s="1" t="s">
-        <v>4714</v>
+        <v>4696</v>
       </c>
     </row>
     <row r="356" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34888,19 +34888,19 @@
         <v>2556</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>4731</v>
+        <v>4710</v>
       </c>
       <c r="D356" t="b">
         <v>1</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>4715</v>
+        <v>4697</v>
       </c>
       <c r="F356">
         <v>1</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34911,19 +34911,19 @@
         <v>2557</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>4732</v>
+        <v>4711</v>
       </c>
       <c r="D357" t="b">
         <v>1</v>
       </c>
       <c r="E357" s="1" t="s">
-        <v>4716</v>
+        <v>4698</v>
       </c>
       <c r="F357">
         <v>2</v>
       </c>
       <c r="G357" s="1" t="s">
-        <v>4717</v>
+        <v>4823</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34934,19 +34934,19 @@
         <v>2558</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>4718</v>
+        <v>4699</v>
       </c>
       <c r="D358" t="b">
         <v>1</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>4719</v>
+        <v>4700</v>
       </c>
       <c r="F358">
         <v>2</v>
       </c>
       <c r="G358" s="1" t="s">
-        <v>4720</v>
+        <v>4824</v>
       </c>
     </row>
     <row r="359" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34957,7 +34957,7 @@
         <v>2559</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>4721</v>
+        <v>4701</v>
       </c>
       <c r="D359" t="b">
         <v>1</v>
@@ -34969,7 +34969,7 @@
         <v>1</v>
       </c>
       <c r="G359" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="360" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34986,7 +34986,7 @@
         <v>0</v>
       </c>
       <c r="E360" s="1" t="s">
-        <v>4722</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="361" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34997,19 +34997,19 @@
         <v>2561</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>4733</v>
+        <v>4712</v>
       </c>
       <c r="D361" t="b">
         <v>1</v>
       </c>
       <c r="E361" s="1" t="s">
-        <v>4734</v>
+        <v>4713</v>
       </c>
       <c r="F361">
         <v>2</v>
       </c>
       <c r="G361" s="1" t="s">
-        <v>4648</v>
+        <v>4637</v>
       </c>
     </row>
     <row r="362" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35020,19 +35020,19 @@
         <v>2562</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>4735</v>
+        <v>4714</v>
       </c>
       <c r="D362" t="b">
         <v>1</v>
       </c>
       <c r="E362" s="1" t="s">
-        <v>4723</v>
+        <v>4703</v>
       </c>
       <c r="F362">
         <v>1</v>
       </c>
       <c r="G362" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="363" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35043,19 +35043,19 @@
         <v>2563</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>4736</v>
+        <v>4715</v>
       </c>
       <c r="D363" t="b">
         <v>1</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>4724</v>
+        <v>4704</v>
       </c>
       <c r="F363">
         <v>2</v>
       </c>
       <c r="G363" s="1" t="s">
-        <v>4593</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -35072,7 +35072,7 @@
         <v>0</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>4722</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="365" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -35083,19 +35083,19 @@
         <v>2565</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>4737</v>
+        <v>4716</v>
       </c>
       <c r="D365" t="b">
         <v>1</v>
       </c>
       <c r="E365" s="1" t="s">
-        <v>4725</v>
+        <v>4705</v>
       </c>
       <c r="F365">
         <v>1</v>
       </c>
       <c r="G365" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="366" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35106,7 +35106,7 @@
         <v>2566</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>4738</v>
+        <v>4717</v>
       </c>
       <c r="D366" t="b">
         <v>1</v>
@@ -35126,7 +35126,7 @@
         <v>2567</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>4739</v>
+        <v>4718</v>
       </c>
       <c r="D367" t="b">
         <v>1</v>
@@ -35138,7 +35138,7 @@
         <v>3</v>
       </c>
       <c r="G367" s="1" t="s">
-        <v>4740</v>
+        <v>4825</v>
       </c>
     </row>
     <row r="368" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35149,19 +35149,19 @@
         <v>2568</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>4741</v>
+        <v>4719</v>
       </c>
       <c r="D368" t="b">
         <v>1</v>
       </c>
       <c r="E368" s="1" t="s">
-        <v>4742</v>
+        <v>4720</v>
       </c>
       <c r="F368">
         <v>1</v>
       </c>
       <c r="G368" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="369" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35172,19 +35172,19 @@
         <v>2569</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>4743</v>
+        <v>4721</v>
       </c>
       <c r="D369" t="b">
         <v>1</v>
       </c>
       <c r="E369" s="1" t="s">
-        <v>4744</v>
+        <v>4722</v>
       </c>
       <c r="F369">
         <v>1</v>
       </c>
       <c r="G369" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="370" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35195,19 +35195,19 @@
         <v>2570</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>4745</v>
+        <v>4723</v>
       </c>
       <c r="D370" t="b">
         <v>1</v>
       </c>
       <c r="E370" s="1" t="s">
-        <v>4746</v>
+        <v>4724</v>
       </c>
       <c r="F370">
         <v>2</v>
       </c>
       <c r="G370" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="371" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35273,19 +35273,19 @@
         <v>2576</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>4747</v>
+        <v>4725</v>
       </c>
       <c r="D376" t="b">
         <v>1</v>
       </c>
       <c r="E376" s="1" t="s">
-        <v>4748</v>
+        <v>4726</v>
       </c>
       <c r="F376">
         <v>3</v>
       </c>
       <c r="G376" s="1" t="s">
-        <v>4749</v>
+        <v>4826</v>
       </c>
     </row>
     <row r="377" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35379,7 +35379,7 @@
         <v>0</v>
       </c>
       <c r="E384" s="1" t="s">
-        <v>4750</v>
+        <v>4727</v>
       </c>
     </row>
     <row r="385" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35412,19 +35412,19 @@
         <v>2587</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>4751</v>
+        <v>4728</v>
       </c>
       <c r="D387" t="b">
         <v>1</v>
       </c>
       <c r="E387" s="1" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="F387">
         <v>1</v>
       </c>
       <c r="G387" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="388" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35435,7 +35435,7 @@
         <v>2588</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>4752</v>
+        <v>4729</v>
       </c>
       <c r="D388" t="b">
         <v>1</v>
@@ -35447,7 +35447,7 @@
         <v>1</v>
       </c>
       <c r="G388" s="1" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="389" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35502,19 +35502,19 @@
         <v>2593</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>4753</v>
+        <v>4730</v>
       </c>
       <c r="D393" t="b">
         <v>1</v>
       </c>
       <c r="E393" s="1" t="s">
-        <v>4754</v>
+        <v>4731</v>
       </c>
       <c r="F393">
         <v>1</v>
       </c>
       <c r="G393" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="394" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35580,19 +35580,19 @@
         <v>2599</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>4755</v>
+        <v>4732</v>
       </c>
       <c r="D399" t="b">
         <v>1</v>
       </c>
       <c r="E399" s="1" t="s">
-        <v>4756</v>
+        <v>4733</v>
       </c>
       <c r="F399">
         <v>2</v>
       </c>
       <c r="G399" s="1" t="s">
-        <v>4757</v>
+        <v>4827</v>
       </c>
     </row>
     <row r="400" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35614,7 +35614,7 @@
         <v>2601</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>4758</v>
+        <v>4734</v>
       </c>
       <c r="D401" t="b">
         <v>1</v>
@@ -35626,7 +35626,7 @@
         <v>2</v>
       </c>
       <c r="G401" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="402" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35659,16 +35659,16 @@
         <v>2604</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>4759</v>
+        <v>4735</v>
       </c>
       <c r="D404" t="b">
         <v>1</v>
       </c>
       <c r="E404" s="1" t="s">
-        <v>4760</v>
+        <v>4736</v>
       </c>
       <c r="F404" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="405" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35679,16 +35679,16 @@
         <v>2605</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>4761</v>
+        <v>4737</v>
       </c>
       <c r="D405" t="b">
         <v>1</v>
       </c>
       <c r="E405" s="1" t="s">
-        <v>4762</v>
+        <v>4738</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>4672</v>
+        <v>4818</v>
       </c>
     </row>
     <row r="406" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35710,16 +35710,16 @@
         <v>2607</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>4763</v>
+        <v>4739</v>
       </c>
       <c r="D407" t="b">
         <v>1</v>
       </c>
       <c r="E407" s="1" t="s">
-        <v>4764</v>
+        <v>4740</v>
       </c>
       <c r="F407" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="408" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -35730,13 +35730,13 @@
         <v>2608</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>4765</v>
+        <v>4741</v>
       </c>
       <c r="D408" t="b">
         <v>1</v>
       </c>
       <c r="E408" s="1" t="s">
-        <v>4766</v>
+        <v>4742</v>
       </c>
       <c r="F408" s="1" t="s">
         <v>4578</v>
@@ -35750,16 +35750,16 @@
         <v>2609</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>4767</v>
+        <v>4743</v>
       </c>
       <c r="D409" t="b">
         <v>1</v>
       </c>
       <c r="E409" s="1" t="s">
-        <v>4768</v>
+        <v>4744</v>
       </c>
       <c r="F409" s="1" t="s">
-        <v>4590</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="410" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35781,7 +35781,7 @@
         <v>2611</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>4769</v>
+        <v>4745</v>
       </c>
       <c r="D411" t="b">
         <v>1</v>
@@ -35790,7 +35790,7 @@
         <v>4462</v>
       </c>
       <c r="F411" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="412" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -35823,19 +35823,19 @@
         <v>2614</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>4770</v>
+        <v>4746</v>
       </c>
       <c r="D414" t="b">
         <v>1</v>
       </c>
       <c r="E414" s="1" t="s">
-        <v>4771</v>
+        <v>4747</v>
       </c>
       <c r="F414">
         <v>2</v>
       </c>
       <c r="G414" s="1" t="s">
-        <v>4772</v>
+        <v>4828</v>
       </c>
     </row>
     <row r="415" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -35846,7 +35846,7 @@
         <v>2615</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>4773</v>
+        <v>4748</v>
       </c>
       <c r="D415" t="b">
         <v>1</v>
@@ -35858,7 +35858,7 @@
         <v>1</v>
       </c>
       <c r="G415" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="416" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35869,19 +35869,19 @@
         <v>2616</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>4774</v>
+        <v>4749</v>
       </c>
       <c r="D416" t="b">
         <v>1</v>
       </c>
       <c r="E416" s="1" t="s">
-        <v>4775</v>
+        <v>4750</v>
       </c>
       <c r="F416">
         <v>1</v>
       </c>
       <c r="G416" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="417" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35953,7 +35953,7 @@
         <v>0</v>
       </c>
       <c r="E422" s="1" t="s">
-        <v>4776</v>
+        <v>4751</v>
       </c>
     </row>
     <row r="423" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -35964,19 +35964,19 @@
         <v>2623</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>4777</v>
+        <v>4752</v>
       </c>
       <c r="D423" t="b">
         <v>1</v>
       </c>
       <c r="E423" s="1" t="s">
-        <v>4778</v>
+        <v>4753</v>
       </c>
       <c r="F423">
         <v>2</v>
       </c>
       <c r="G423" s="1" t="s">
-        <v>4589</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="424" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -36031,7 +36031,7 @@
         <v>2628</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>4779</v>
+        <v>4754</v>
       </c>
       <c r="D428" t="b">
         <v>1</v>
@@ -36043,7 +36043,7 @@
         <v>1</v>
       </c>
       <c r="G428" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="429" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36054,19 +36054,19 @@
         <v>2629</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>4780</v>
+        <v>4755</v>
       </c>
       <c r="D429" t="b">
         <v>1</v>
       </c>
       <c r="E429" s="1" t="s">
-        <v>4639</v>
+        <v>4628</v>
       </c>
       <c r="F429">
         <v>2</v>
       </c>
       <c r="G429" s="1" t="s">
-        <v>4708</v>
+        <v>4821</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -36105,7 +36105,7 @@
         <v>0</v>
       </c>
       <c r="E432" s="1" t="s">
-        <v>4781</v>
+        <v>4756</v>
       </c>
     </row>
     <row r="433" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -36116,13 +36116,13 @@
         <v>2633</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>4782</v>
+        <v>4757</v>
       </c>
       <c r="D433" t="b">
         <v>1</v>
       </c>
       <c r="E433" s="1" t="s">
-        <v>4783</v>
+        <v>4758</v>
       </c>
       <c r="F433">
         <v>1</v>
@@ -36161,19 +36161,19 @@
         <v>2636</v>
       </c>
       <c r="C436" s="1" t="s">
-        <v>4784</v>
+        <v>4759</v>
       </c>
       <c r="D436" t="b">
         <v>1</v>
       </c>
       <c r="E436" s="1" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="F436">
         <v>1</v>
       </c>
       <c r="G436" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="437" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36195,7 +36195,7 @@
         <v>2638</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>4785</v>
+        <v>4760</v>
       </c>
       <c r="D438" t="b">
         <v>1</v>
@@ -36207,7 +36207,7 @@
         <v>1</v>
       </c>
       <c r="G438" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="439" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36218,13 +36218,13 @@
         <v>2639</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>4786</v>
+        <v>4761</v>
       </c>
       <c r="D439" t="b">
         <v>1</v>
       </c>
       <c r="E439" s="1" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="F439">
         <v>1</v>
@@ -36285,19 +36285,19 @@
         <v>2644</v>
       </c>
       <c r="C444" s="1" t="s">
-        <v>4787</v>
+        <v>4762</v>
       </c>
       <c r="D444" t="b">
         <v>1</v>
       </c>
       <c r="E444" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F444">
         <v>1</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="445" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36308,19 +36308,19 @@
         <v>2645</v>
       </c>
       <c r="C445" s="1" t="s">
-        <v>4788</v>
+        <v>4763</v>
       </c>
       <c r="D445" t="b">
         <v>1</v>
       </c>
       <c r="E445" s="1" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="F445" s="1">
         <v>1</v>
       </c>
       <c r="G445" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="446" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36353,7 +36353,7 @@
         <v>2648</v>
       </c>
       <c r="C448" s="1" t="s">
-        <v>4789</v>
+        <v>4764</v>
       </c>
       <c r="D448" t="b">
         <v>1</v>
@@ -36365,7 +36365,7 @@
         <v>1</v>
       </c>
       <c r="G448" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="449" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -36387,19 +36387,19 @@
         <v>2650</v>
       </c>
       <c r="C450" s="1" t="s">
-        <v>4790</v>
+        <v>4765</v>
       </c>
       <c r="D450" t="b">
         <v>1</v>
       </c>
       <c r="E450" s="1" t="s">
-        <v>4791</v>
+        <v>4766</v>
       </c>
       <c r="F450">
         <v>1</v>
       </c>
       <c r="G450" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="451" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36471,7 +36471,7 @@
         <v>0</v>
       </c>
       <c r="E456" s="1" t="s">
-        <v>4792</v>
+        <v>4767</v>
       </c>
     </row>
     <row r="457" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36526,19 +36526,19 @@
         <v>2661</v>
       </c>
       <c r="C461" s="1" t="s">
-        <v>4793</v>
+        <v>4768</v>
       </c>
       <c r="D461" t="b">
         <v>1</v>
       </c>
       <c r="E461" s="1" t="s">
-        <v>4794</v>
+        <v>4769</v>
       </c>
       <c r="F461">
         <v>1</v>
       </c>
       <c r="G461" s="1" t="s">
-        <v>4596</v>
+        <v>4804</v>
       </c>
     </row>
     <row r="462" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36725,19 +36725,19 @@
         <v>2678</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>4795</v>
+        <v>4770</v>
       </c>
       <c r="D478" t="b">
         <v>1</v>
       </c>
       <c r="E478" s="1" t="s">
-        <v>4796</v>
+        <v>4771</v>
       </c>
       <c r="F478">
         <v>1</v>
       </c>
       <c r="G478" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="479" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -36781,19 +36781,19 @@
         <v>2682</v>
       </c>
       <c r="C482" s="1" t="s">
-        <v>4797</v>
+        <v>4772</v>
       </c>
       <c r="D482" t="b">
         <v>1</v>
       </c>
       <c r="E482" s="1" t="s">
-        <v>4798</v>
+        <v>4773</v>
       </c>
       <c r="F482">
         <v>1</v>
       </c>
       <c r="G482" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="483" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36865,7 +36865,7 @@
         <v>0</v>
       </c>
       <c r="E488" s="1" t="s">
-        <v>4792</v>
+        <v>4767</v>
       </c>
     </row>
     <row r="489" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36915,7 +36915,7 @@
         <v>0</v>
       </c>
       <c r="E492" s="1" t="s">
-        <v>4799</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="493" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36943,7 +36943,7 @@
         <v>0</v>
       </c>
       <c r="E494" s="1" t="s">
-        <v>4799</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="495" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37020,19 +37020,19 @@
         <v>2701</v>
       </c>
       <c r="C501" s="1" t="s">
-        <v>4800</v>
+        <v>4775</v>
       </c>
       <c r="D501" t="b">
         <v>1</v>
       </c>
       <c r="E501" s="1" t="s">
-        <v>4801</v>
+        <v>4776</v>
       </c>
       <c r="F501">
         <v>2</v>
       </c>
       <c r="G501" s="1" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="502" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37071,7 +37071,7 @@
         <v>0</v>
       </c>
       <c r="E504" s="1" t="s">
-        <v>4799</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="505" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -37082,19 +37082,19 @@
         <v>2705</v>
       </c>
       <c r="C505" s="1" t="s">
-        <v>4802</v>
+        <v>4777</v>
       </c>
       <c r="D505" t="b">
         <v>1</v>
       </c>
       <c r="E505" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F505">
         <v>1</v>
       </c>
       <c r="G505" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="506" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37116,7 +37116,7 @@
         <v>2707</v>
       </c>
       <c r="C507" s="1" t="s">
-        <v>4803</v>
+        <v>4778</v>
       </c>
       <c r="D507" t="b">
         <v>1</v>
@@ -37128,7 +37128,7 @@
         <v>1</v>
       </c>
       <c r="G507" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="508" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37161,19 +37161,19 @@
         <v>2710</v>
       </c>
       <c r="C510" s="1" t="s">
-        <v>4804</v>
+        <v>4779</v>
       </c>
       <c r="D510" t="b">
         <v>1</v>
       </c>
       <c r="E510" s="1" t="s">
-        <v>4766</v>
+        <v>4742</v>
       </c>
       <c r="F510">
         <v>1</v>
       </c>
       <c r="G510" s="1" t="s">
-        <v>4591</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="511" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37184,7 +37184,7 @@
         <v>2711</v>
       </c>
       <c r="C511" s="1" t="s">
-        <v>4805</v>
+        <v>4780</v>
       </c>
       <c r="D511" t="b">
         <v>1</v>
@@ -37196,7 +37196,7 @@
         <v>1</v>
       </c>
       <c r="G511" s="1" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="512" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37207,7 +37207,7 @@
         <v>2712</v>
       </c>
       <c r="C512" s="1" t="s">
-        <v>4806</v>
+        <v>4781</v>
       </c>
       <c r="D512" t="b">
         <v>1</v>
@@ -37318,7 +37318,7 @@
         <v>2721</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>4829</v>
+        <v>4803</v>
       </c>
       <c r="D521" t="b">
         <v>1</v>
@@ -37330,7 +37330,7 @@
         <v>2</v>
       </c>
       <c r="G521" s="1" t="s">
-        <v>4708</v>
+        <v>4821</v>
       </c>
     </row>
     <row r="522" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37363,19 +37363,19 @@
         <v>2724</v>
       </c>
       <c r="C524" s="1" t="s">
-        <v>4807</v>
+        <v>4782</v>
       </c>
       <c r="D524" t="b">
         <v>1</v>
       </c>
       <c r="E524" s="1" t="s">
-        <v>4808</v>
+        <v>4783</v>
       </c>
       <c r="F524">
         <v>1</v>
       </c>
       <c r="G524" s="1" t="s">
-        <v>4595</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="525" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37403,7 +37403,7 @@
         <v>0</v>
       </c>
       <c r="E526" s="1" t="s">
-        <v>4799</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="527" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -37436,13 +37436,13 @@
         <v>2729</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>4828</v>
+        <v>4802</v>
       </c>
       <c r="D529" t="b">
         <v>1</v>
       </c>
       <c r="E529" s="1" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="F529">
         <v>1</v>
@@ -37470,19 +37470,19 @@
         <v>2731</v>
       </c>
       <c r="C531" s="1" t="s">
-        <v>4825</v>
+        <v>4799</v>
       </c>
       <c r="D531" t="b">
         <v>1</v>
       </c>
       <c r="E531" s="1" t="s">
-        <v>4826</v>
+        <v>4800</v>
       </c>
       <c r="F531" s="1">
         <v>1</v>
       </c>
       <c r="G531" s="1" t="s">
-        <v>4827</v>
+        <v>4801</v>
       </c>
     </row>
     <row r="532" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37504,7 +37504,7 @@
         <v>2733</v>
       </c>
       <c r="C533" s="1" t="s">
-        <v>4809</v>
+        <v>4784</v>
       </c>
       <c r="D533" t="b">
         <v>1</v>
@@ -37516,7 +37516,7 @@
         <v>2</v>
       </c>
       <c r="G533" s="1" t="s">
-        <v>4810</v>
+        <v>4785</v>
       </c>
     </row>
     <row r="534" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37538,19 +37538,19 @@
         <v>2735</v>
       </c>
       <c r="C535" s="1" t="s">
-        <v>4811</v>
+        <v>4786</v>
       </c>
       <c r="D535" t="b">
         <v>1</v>
       </c>
       <c r="E535" s="1" t="s">
-        <v>4812</v>
+        <v>4787</v>
       </c>
       <c r="F535">
         <v>1</v>
       </c>
       <c r="G535" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="536" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37572,19 +37572,19 @@
         <v>2737</v>
       </c>
       <c r="C537" s="1" t="s">
-        <v>4813</v>
+        <v>4788</v>
       </c>
       <c r="D537" t="b">
         <v>1</v>
       </c>
       <c r="E537" s="1" t="s">
-        <v>4812</v>
+        <v>4787</v>
       </c>
       <c r="F537">
         <v>1</v>
       </c>
       <c r="G537" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="538" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37606,19 +37606,19 @@
         <v>2739</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>4814</v>
+        <v>4789</v>
       </c>
       <c r="D539" t="b">
         <v>1</v>
       </c>
       <c r="E539" s="1" t="s">
-        <v>4812</v>
+        <v>4787</v>
       </c>
       <c r="F539">
         <v>1</v>
       </c>
       <c r="G539" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="540" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37640,19 +37640,19 @@
         <v>2741</v>
       </c>
       <c r="C541" s="1" t="s">
-        <v>4815</v>
+        <v>4790</v>
       </c>
       <c r="D541" t="b">
         <v>1</v>
       </c>
       <c r="E541" s="1" t="s">
-        <v>4812</v>
+        <v>4787</v>
       </c>
       <c r="F541">
         <v>1</v>
       </c>
       <c r="G541" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="542" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -37663,7 +37663,7 @@
         <v>2742</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>4816</v>
+        <v>4791</v>
       </c>
       <c r="D542" t="b">
         <v>1</v>
@@ -37675,7 +37675,7 @@
         <v>2</v>
       </c>
       <c r="G542" s="1" t="s">
-        <v>4817</v>
+        <v>4829</v>
       </c>
     </row>
     <row r="543" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37697,19 +37697,19 @@
         <v>2744</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>4818</v>
+        <v>4792</v>
       </c>
       <c r="D544" t="b">
         <v>1</v>
       </c>
       <c r="E544" s="1" t="s">
-        <v>4650</v>
+        <v>4639</v>
       </c>
       <c r="F544">
         <v>1</v>
       </c>
       <c r="G544" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37720,19 +37720,19 @@
         <v>2745</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>4819</v>
+        <v>4793</v>
       </c>
       <c r="D545" t="b">
         <v>1</v>
       </c>
       <c r="E545" s="1" t="s">
-        <v>4820</v>
+        <v>4794</v>
       </c>
       <c r="F545">
         <v>2</v>
       </c>
       <c r="G545" s="1" t="s">
-        <v>4594</v>
+        <v>4807</v>
       </c>
     </row>
     <row r="546" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37743,7 +37743,7 @@
         <v>2746</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>4821</v>
+        <v>4795</v>
       </c>
       <c r="D546" t="b">
         <v>1</v>
@@ -37755,7 +37755,7 @@
         <v>1</v>
       </c>
       <c r="G546" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="547" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37766,19 +37766,19 @@
         <v>2747</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>4822</v>
+        <v>4796</v>
       </c>
       <c r="D547" t="b">
         <v>1</v>
       </c>
       <c r="E547" s="1" t="s">
-        <v>4812</v>
+        <v>4787</v>
       </c>
       <c r="F547">
         <v>2</v>
       </c>
       <c r="G547" s="1" t="s">
-        <v>4583</v>
+        <v>4815</v>
       </c>
     </row>
     <row r="548" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -37789,7 +37789,7 @@
         <v>2748</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>4823</v>
+        <v>4797</v>
       </c>
       <c r="D548" t="b">
         <v>1</v>
@@ -37801,7 +37801,7 @@
         <v>1</v>
       </c>
       <c r="G548" s="1" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="549" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37812,7 +37812,7 @@
         <v>2749</v>
       </c>
       <c r="C549" s="1" t="s">
-        <v>4824</v>
+        <v>4798</v>
       </c>
       <c r="D549" t="b">
         <v>1</v>
@@ -37824,7 +37824,7 @@
         <v>1</v>
       </c>
       <c r="G549" s="1" t="s">
-        <v>4585</v>
+        <v>4583</v>
       </c>
     </row>
     <row r="550" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37841,7 +37841,7 @@
         <v>0</v>
       </c>
       <c r="E550" s="1" t="s">
-        <v>4799</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="551" spans="1:7" ht="176" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add more leh51 labels and clean conversations
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
+++ b/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51146EF9-DE8A-5E44-BD71-00C323553054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D91A9BA-76A9-4A4A-87AD-CDBC6EB7BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="singlish_NUS_SMS" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7168" uniqueCount="4830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7188" uniqueCount="4844">
   <si>
     <t>original_sentence</t>
   </si>
@@ -28812,6 +28812,89 @@
   </si>
   <si>
     <t>["lor33", "leh33"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Mei, what do you want to eat for dinner tonight?
+B: Don’t know leh
+A: Everyday don’t know leh don’t know leh, you go out eat yourself lah</t>
+  </si>
+  <si>
+    <t>["leh33", "leh51", "leh51", "lah51"]</t>
+  </si>
+  <si>
+    <t>balance dataset, edit to fit leh51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: You submitted your assignment late?
+B: Ya, I emailed to ask the prof leh and he gave me the wrong date 
+A: Are you serious?
+B: Yah, I'm so pissed, I wrote in again to clarify and he ignored my further emails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: She's the best at dancing leh
+B: Really? 
+A: Yes, she's really really good. 
+B: okay, maybe I'll talk to her and pull her to my hall dance team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Wah, girl's shouldn't be going out to work, only cause me trouble
+B: You very sexist leh
+A: What????
+B: I cannot be bothered to talk to you, can't believe we were friends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Wah, that guy super slow leh, everyone leave already, I don't understand how can he be so slow
+B: Should we just leave first? I think he said he needs another half an hour or so
+A: Haiz, okay let's leave first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Oh no, I forgot my phone at home.
+B: Haiyoh! You are very blur leh
+A: Yeah, I'm sometimes forgetful
+B: It's too late to go back, don’t worry, I'll lend you mine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Have you submitted your university acceptance form?
+B: Huh, no, when is it due?
+A: You must hand it in by the 24th.
+B: Oh, okay. Wait, why is it due so early?
+A: Our matriculation is on the 29th, you know.
+B: Oh, I see. That makes sense.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Bank robbery leh, and you dare to tackle the robbers?
+B: Yeah, adrenaline rush haha
+A: You not scared?
+B: I don’t know, before my brain even processed anything, my body already kicked the robber oops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Hey, are you coming to the party tonight?
+B: Yeah, I'll be there. But I might be a little late.
+A: The party has already started. You very late leh
+B: Sorry Sorry, I'm really reaching</t>
+  </si>
+  <si>
+    <t>A: Wah should I offer tuition again? This parent offering me $200 leh
+B: What? 200? So much?
+A: Ya, more than double the market rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: my friend just got a full time offer from this AI company 
+B: Really? This company is damn hard to get in leh
+A: Oh, I didn't even know haha he is smart lah</t>
+  </si>
+  <si>
+    <t>["leh51", "lah21"]</t>
   </si>
 </sst>
 </file>
@@ -29219,9 +29302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A934" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B936" sqref="B936"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38482,7 +38565,7 @@
         <v>2808</v>
       </c>
     </row>
-    <row r="609" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A609" s="1" t="s">
         <v>582</v>
       </c>
@@ -38493,7 +38576,7 @@
         <v>2809</v>
       </c>
     </row>
-    <row r="610" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
         <v>583</v>
       </c>
@@ -38504,7 +38587,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="611" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A611" s="1" t="s">
         <v>584</v>
       </c>
@@ -38515,7 +38598,7 @@
         <v>2811</v>
       </c>
     </row>
-    <row r="612" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A612" s="1" t="s">
         <v>585</v>
       </c>
@@ -38526,7 +38609,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="613" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A613" s="1" t="s">
         <v>586</v>
       </c>
@@ -38537,7 +38620,7 @@
         <v>2813</v>
       </c>
     </row>
-    <row r="614" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A614" s="1" t="s">
         <v>587</v>
       </c>
@@ -38548,7 +38631,7 @@
         <v>2814</v>
       </c>
     </row>
-    <row r="615" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A615" s="1" t="s">
         <v>588</v>
       </c>
@@ -38559,7 +38642,7 @@
         <v>2815</v>
       </c>
     </row>
-    <row r="616" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A616" s="1" t="s">
         <v>589</v>
       </c>
@@ -38570,7 +38653,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="617" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A617" s="1" t="s">
         <v>590</v>
       </c>
@@ -38581,7 +38664,7 @@
         <v>2817</v>
       </c>
     </row>
-    <row r="618" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A618" s="1" t="s">
         <v>591</v>
       </c>
@@ -38592,7 +38675,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="619" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A619" s="1" t="s">
         <v>592</v>
       </c>
@@ -38603,7 +38686,7 @@
         <v>2819</v>
       </c>
     </row>
-    <row r="620" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A620" s="1" t="s">
         <v>593</v>
       </c>
@@ -38614,7 +38697,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="621" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A621" s="1" t="s">
         <v>594</v>
       </c>
@@ -38622,10 +38705,22 @@
         <v>2821</v>
       </c>
       <c r="C621" s="1" t="s">
-        <v>2821</v>
-      </c>
-    </row>
-    <row r="622" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+        <v>4830</v>
+      </c>
+      <c r="D621" t="b">
+        <v>1</v>
+      </c>
+      <c r="E621" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F621">
+        <v>4</v>
+      </c>
+      <c r="G621" s="1" t="s">
+        <v>4831</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A622" s="1" t="s">
         <v>595</v>
       </c>
@@ -38636,7 +38731,7 @@
         <v>2822</v>
       </c>
     </row>
-    <row r="623" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A623" s="1" t="s">
         <v>596</v>
       </c>
@@ -38647,7 +38742,7 @@
         <v>2823</v>
       </c>
     </row>
-    <row r="624" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
         <v>597</v>
       </c>
@@ -38658,7 +38753,7 @@
         <v>2824</v>
       </c>
     </row>
-    <row r="625" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A625" s="1" t="s">
         <v>598</v>
       </c>
@@ -38669,7 +38764,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="626" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A626" s="1" t="s">
         <v>599</v>
       </c>
@@ -38677,10 +38772,19 @@
         <v>2826</v>
       </c>
       <c r="C626" s="1" t="s">
-        <v>2826</v>
-      </c>
-    </row>
-    <row r="627" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+        <v>4833</v>
+      </c>
+      <c r="D626" t="b">
+        <v>1</v>
+      </c>
+      <c r="E626" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F626" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A627" s="1" t="s">
         <v>600</v>
       </c>
@@ -38691,7 +38795,7 @@
         <v>2827</v>
       </c>
     </row>
-    <row r="628" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A628" s="1" t="s">
         <v>601</v>
       </c>
@@ -38702,7 +38806,7 @@
         <v>2828</v>
       </c>
     </row>
-    <row r="629" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A629" s="1" t="s">
         <v>602</v>
       </c>
@@ -38713,7 +38817,7 @@
         <v>2829</v>
       </c>
     </row>
-    <row r="630" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A630" s="1" t="s">
         <v>603</v>
       </c>
@@ -38724,7 +38828,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="631" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A631" s="1" t="s">
         <v>604</v>
       </c>
@@ -38735,7 +38839,7 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="632" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="632" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A632" s="1" t="s">
         <v>605</v>
       </c>
@@ -38746,7 +38850,7 @@
         <v>2832</v>
       </c>
     </row>
-    <row r="633" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="633" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A633" s="1" t="s">
         <v>606</v>
       </c>
@@ -38757,7 +38861,7 @@
         <v>2833</v>
       </c>
     </row>
-    <row r="634" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A634" s="1" t="s">
         <v>607</v>
       </c>
@@ -38768,7 +38872,7 @@
         <v>2834</v>
       </c>
     </row>
-    <row r="635" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A635" s="1" t="s">
         <v>608</v>
       </c>
@@ -38779,7 +38883,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="636" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A636" s="1" t="s">
         <v>609</v>
       </c>
@@ -38790,7 +38894,7 @@
         <v>2836</v>
       </c>
     </row>
-    <row r="637" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A637" s="1" t="s">
         <v>610</v>
       </c>
@@ -38801,7 +38905,7 @@
         <v>2837</v>
       </c>
     </row>
-    <row r="638" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A638" s="1" t="s">
         <v>611</v>
       </c>
@@ -38812,7 +38916,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="639" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A639" s="1" t="s">
         <v>612</v>
       </c>
@@ -38823,7 +38927,7 @@
         <v>2839</v>
       </c>
     </row>
-    <row r="640" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A640" s="1" t="s">
         <v>613</v>
       </c>
@@ -39186,7 +39290,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="673" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="673" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A673" s="1" t="s">
         <v>646</v>
       </c>
@@ -39197,7 +39301,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="674" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+    <row r="674" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A674" s="1" t="s">
         <v>647</v>
       </c>
@@ -39208,7 +39312,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="675" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="675" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A675" s="1" t="s">
         <v>648</v>
       </c>
@@ -39219,7 +39323,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="676" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A676" s="1" t="s">
         <v>649</v>
       </c>
@@ -39230,7 +39334,7 @@
         <v>2876</v>
       </c>
     </row>
-    <row r="677" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+    <row r="677" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A677" s="1" t="s">
         <v>650</v>
       </c>
@@ -39238,10 +39342,19 @@
         <v>2877</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>2877</v>
-      </c>
-    </row>
-    <row r="678" spans="1:3" ht="208" x14ac:dyDescent="0.2">
+        <v>4834</v>
+      </c>
+      <c r="D677" t="b">
+        <v>1</v>
+      </c>
+      <c r="E677" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F677" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="678" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A678" s="1" t="s">
         <v>651</v>
       </c>
@@ -39252,7 +39365,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="679" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="679" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A679" s="1" t="s">
         <v>652</v>
       </c>
@@ -39263,7 +39376,7 @@
         <v>2879</v>
       </c>
     </row>
-    <row r="680" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="680" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A680" s="1" t="s">
         <v>653</v>
       </c>
@@ -39274,7 +39387,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="681" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="681" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A681" s="1" t="s">
         <v>654</v>
       </c>
@@ -39285,7 +39398,7 @@
         <v>2881</v>
       </c>
     </row>
-    <row r="682" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="682" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A682" s="1" t="s">
         <v>655</v>
       </c>
@@ -39296,7 +39409,7 @@
         <v>2882</v>
       </c>
     </row>
-    <row r="683" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="683" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A683" s="1" t="s">
         <v>656</v>
       </c>
@@ -39307,7 +39420,7 @@
         <v>2883</v>
       </c>
     </row>
-    <row r="684" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="684" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A684" s="1" t="s">
         <v>657</v>
       </c>
@@ -39318,7 +39431,7 @@
         <v>2884</v>
       </c>
     </row>
-    <row r="685" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+    <row r="685" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A685" s="1" t="s">
         <v>658</v>
       </c>
@@ -39329,7 +39442,7 @@
         <v>2885</v>
       </c>
     </row>
-    <row r="686" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A686" s="1" t="s">
         <v>659</v>
       </c>
@@ -39340,7 +39453,7 @@
         <v>2886</v>
       </c>
     </row>
-    <row r="687" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A687" s="1" t="s">
         <v>660</v>
       </c>
@@ -39351,7 +39464,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="688" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A688" s="1" t="s">
         <v>661</v>
       </c>
@@ -39714,7 +39827,7 @@
         <v>2920</v>
       </c>
     </row>
-    <row r="721" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="721" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A721" s="1" t="s">
         <v>694</v>
       </c>
@@ -39725,7 +39838,7 @@
         <v>2921</v>
       </c>
     </row>
-    <row r="722" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="722" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A722" s="1" t="s">
         <v>695</v>
       </c>
@@ -39736,7 +39849,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="723" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="723" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A723" s="1" t="s">
         <v>696</v>
       </c>
@@ -39747,7 +39860,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="724" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="724" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A724" s="1" t="s">
         <v>697</v>
       </c>
@@ -39758,7 +39871,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="725" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="725" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A725" s="1" t="s">
         <v>698</v>
       </c>
@@ -39769,7 +39882,7 @@
         <v>2925</v>
       </c>
     </row>
-    <row r="726" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="726" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A726" s="1" t="s">
         <v>699</v>
       </c>
@@ -39780,7 +39893,7 @@
         <v>2926</v>
       </c>
     </row>
-    <row r="727" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="727" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A727" s="1" t="s">
         <v>700</v>
       </c>
@@ -39791,7 +39904,7 @@
         <v>2927</v>
       </c>
     </row>
-    <row r="728" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="728" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A728" s="1" t="s">
         <v>701</v>
       </c>
@@ -39802,7 +39915,7 @@
         <v>2928</v>
       </c>
     </row>
-    <row r="729" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A729" s="1" t="s">
         <v>702</v>
       </c>
@@ -39813,7 +39926,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="730" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="730" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A730" s="1" t="s">
         <v>703</v>
       </c>
@@ -39824,7 +39937,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="731" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="731" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A731" s="1" t="s">
         <v>704</v>
       </c>
@@ -39832,10 +39945,19 @@
         <v>2931</v>
       </c>
       <c r="C731" s="1" t="s">
-        <v>2931</v>
-      </c>
-    </row>
-    <row r="732" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>4835</v>
+      </c>
+      <c r="D731" t="b">
+        <v>1</v>
+      </c>
+      <c r="E731" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F731" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="732" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A732" s="1" t="s">
         <v>705</v>
       </c>
@@ -39846,7 +39968,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="733" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="733" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A733" s="1" t="s">
         <v>706</v>
       </c>
@@ -39857,7 +39979,7 @@
         <v>2933</v>
       </c>
     </row>
-    <row r="734" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="734" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A734" s="1" t="s">
         <v>707</v>
       </c>
@@ -39868,7 +39990,7 @@
         <v>2934</v>
       </c>
     </row>
-    <row r="735" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="735" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A735" s="1" t="s">
         <v>708</v>
       </c>
@@ -39876,10 +39998,19 @@
         <v>2935</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>2935</v>
-      </c>
-    </row>
-    <row r="736" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+        <v>4836</v>
+      </c>
+      <c r="D735" t="b">
+        <v>1</v>
+      </c>
+      <c r="E735" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F735" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="736" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A736" s="1" t="s">
         <v>709</v>
       </c>
@@ -40066,7 +40197,7 @@
         <v>2952</v>
       </c>
     </row>
-    <row r="753" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A753" s="1" t="s">
         <v>725</v>
       </c>
@@ -40077,7 +40208,7 @@
         <v>2953</v>
       </c>
     </row>
-    <row r="754" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="754" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A754" s="1" t="s">
         <v>726</v>
       </c>
@@ -40088,7 +40219,7 @@
         <v>2954</v>
       </c>
     </row>
-    <row r="755" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="755" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A755" s="1" t="s">
         <v>727</v>
       </c>
@@ -40099,7 +40230,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="756" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="756" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A756" s="1" t="s">
         <v>728</v>
       </c>
@@ -40110,7 +40241,7 @@
         <v>2956</v>
       </c>
     </row>
-    <row r="757" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="757" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A757" s="1" t="s">
         <v>729</v>
       </c>
@@ -40121,7 +40252,7 @@
         <v>2957</v>
       </c>
     </row>
-    <row r="758" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="758" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A758" s="1" t="s">
         <v>730</v>
       </c>
@@ -40132,7 +40263,7 @@
         <v>2958</v>
       </c>
     </row>
-    <row r="759" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="759" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A759" s="1" t="s">
         <v>731</v>
       </c>
@@ -40140,10 +40271,19 @@
         <v>2959</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>2959</v>
-      </c>
-    </row>
-    <row r="760" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+        <v>4837</v>
+      </c>
+      <c r="D759" t="b">
+        <v>1</v>
+      </c>
+      <c r="E759" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F759" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="760" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A760" s="1" t="s">
         <v>732</v>
       </c>
@@ -40154,7 +40294,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="761" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A761" s="1" t="s">
         <v>733</v>
       </c>
@@ -40165,7 +40305,7 @@
         <v>2961</v>
       </c>
     </row>
-    <row r="762" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="762" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A762" s="1" t="s">
         <v>734</v>
       </c>
@@ -40176,7 +40316,7 @@
         <v>2962</v>
       </c>
     </row>
-    <row r="763" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="763" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A763" s="1" t="s">
         <v>735</v>
       </c>
@@ -40187,7 +40327,7 @@
         <v>2963</v>
       </c>
     </row>
-    <row r="764" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="764" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A764" s="1" t="s">
         <v>736</v>
       </c>
@@ -40198,7 +40338,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="765" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="765" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A765" s="1" t="s">
         <v>737</v>
       </c>
@@ -40209,7 +40349,7 @@
         <v>2965</v>
       </c>
     </row>
-    <row r="766" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="766" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A766" s="1" t="s">
         <v>738</v>
       </c>
@@ -40220,7 +40360,7 @@
         <v>2966</v>
       </c>
     </row>
-    <row r="767" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="767" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A767" s="1" t="s">
         <v>739</v>
       </c>
@@ -40231,7 +40371,7 @@
         <v>2967</v>
       </c>
     </row>
-    <row r="768" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A768" s="1" t="s">
         <v>740</v>
       </c>
@@ -40239,7 +40379,7 @@
         <v>2968</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>2968</v>
+        <v>4838</v>
       </c>
     </row>
     <row r="769" spans="1:3" ht="128" x14ac:dyDescent="0.2">
@@ -40594,7 +40734,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="801" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="801" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A801" s="1" t="s">
         <v>773</v>
       </c>
@@ -40605,7 +40745,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="802" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A802" s="1" t="s">
         <v>774</v>
       </c>
@@ -40616,7 +40756,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="803" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="803" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A803" s="1" t="s">
         <v>775</v>
       </c>
@@ -40627,7 +40767,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="804" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A804" s="1" t="s">
         <v>776</v>
       </c>
@@ -40638,7 +40778,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="805" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="805" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A805" s="1" t="s">
         <v>777</v>
       </c>
@@ -40649,7 +40789,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row r="806" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="806" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A806" s="1" t="s">
         <v>778</v>
       </c>
@@ -40660,7 +40800,7 @@
         <v>3006</v>
       </c>
     </row>
-    <row r="807" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="807" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A807" s="1" t="s">
         <v>779</v>
       </c>
@@ -40671,7 +40811,7 @@
         <v>3007</v>
       </c>
     </row>
-    <row r="808" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="808" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A808" s="1" t="s">
         <v>780</v>
       </c>
@@ -40682,7 +40822,7 @@
         <v>3008</v>
       </c>
     </row>
-    <row r="809" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="809" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A809" s="1" t="s">
         <v>781</v>
       </c>
@@ -40690,10 +40830,19 @@
         <v>3009</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>3009</v>
-      </c>
-    </row>
-    <row r="810" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+        <v>4839</v>
+      </c>
+      <c r="D809" t="b">
+        <v>1</v>
+      </c>
+      <c r="E809" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F809" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="810" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A810" s="1" t="s">
         <v>782</v>
       </c>
@@ -40704,7 +40853,7 @@
         <v>3010</v>
       </c>
     </row>
-    <row r="811" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="811" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A811" s="1" t="s">
         <v>783</v>
       </c>
@@ -40712,10 +40861,19 @@
         <v>3011</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>3011</v>
-      </c>
-    </row>
-    <row r="812" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+        <v>4840</v>
+      </c>
+      <c r="D811" t="b">
+        <v>1</v>
+      </c>
+      <c r="E811" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F811" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="812" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A812" s="1" t="s">
         <v>784</v>
       </c>
@@ -40726,7 +40884,7 @@
         <v>3012</v>
       </c>
     </row>
-    <row r="813" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="813" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A813" s="1" t="s">
         <v>785</v>
       </c>
@@ -40737,7 +40895,7 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="814" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A814" s="1" t="s">
         <v>786</v>
       </c>
@@ -40748,7 +40906,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="815" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="815" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A815" s="1" t="s">
         <v>787</v>
       </c>
@@ -40759,7 +40917,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="816" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="816" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A816" s="1" t="s">
         <v>788</v>
       </c>
@@ -41298,7 +41456,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="865" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A865" s="1" t="s">
         <v>835</v>
       </c>
@@ -41309,7 +41467,7 @@
         <v>3065</v>
       </c>
     </row>
-    <row r="866" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+    <row r="866" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A866" s="1" t="s">
         <v>836</v>
       </c>
@@ -41320,7 +41478,7 @@
         <v>3066</v>
       </c>
     </row>
-    <row r="867" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="867" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A867" s="1" t="s">
         <v>647</v>
       </c>
@@ -41331,7 +41489,7 @@
         <v>3067</v>
       </c>
     </row>
-    <row r="868" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="868" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A868" s="1" t="s">
         <v>837</v>
       </c>
@@ -41342,7 +41500,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="869" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="869" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A869" s="1" t="s">
         <v>838</v>
       </c>
@@ -41353,7 +41511,7 @@
         <v>3069</v>
       </c>
     </row>
-    <row r="870" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="870" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A870" s="1" t="s">
         <v>839</v>
       </c>
@@ -41364,7 +41522,7 @@
         <v>3070</v>
       </c>
     </row>
-    <row r="871" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="871" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A871" s="1" t="s">
         <v>840</v>
       </c>
@@ -41375,7 +41533,7 @@
         <v>3071</v>
       </c>
     </row>
-    <row r="872" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="872" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A872" s="1" t="s">
         <v>841</v>
       </c>
@@ -41386,7 +41544,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="873" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="873" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A873" s="1" t="s">
         <v>842</v>
       </c>
@@ -41397,7 +41555,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="874" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="874" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A874" s="1" t="s">
         <v>843</v>
       </c>
@@ -41408,7 +41566,7 @@
         <v>3074</v>
       </c>
     </row>
-    <row r="875" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="875" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A875" s="1" t="s">
         <v>844</v>
       </c>
@@ -41416,10 +41574,19 @@
         <v>3075</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>3075</v>
-      </c>
-    </row>
-    <row r="876" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+        <v>4841</v>
+      </c>
+      <c r="D875" t="b">
+        <v>1</v>
+      </c>
+      <c r="E875" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F875" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="876" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A876" s="1" t="s">
         <v>845</v>
       </c>
@@ -41430,7 +41597,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="877" spans="1:3" ht="224" x14ac:dyDescent="0.2">
+    <row r="877" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A877" s="1" t="s">
         <v>846</v>
       </c>
@@ -41441,7 +41608,7 @@
         <v>3077</v>
       </c>
     </row>
-    <row r="878" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="878" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A878" s="1" t="s">
         <v>847</v>
       </c>
@@ -41452,7 +41619,7 @@
         <v>3078</v>
       </c>
     </row>
-    <row r="879" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="879" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A879" s="1" t="s">
         <v>848</v>
       </c>
@@ -41463,7 +41630,7 @@
         <v>3079</v>
       </c>
     </row>
-    <row r="880" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="880" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A880" s="1" t="s">
         <v>849</v>
       </c>
@@ -42002,7 +42169,7 @@
         <v>3128</v>
       </c>
     </row>
-    <row r="929" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="929" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A929" s="1" t="s">
         <v>896</v>
       </c>
@@ -42013,7 +42180,7 @@
         <v>3129</v>
       </c>
     </row>
-    <row r="930" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+    <row r="930" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A930" s="1" t="s">
         <v>897</v>
       </c>
@@ -42024,7 +42191,7 @@
         <v>3130</v>
       </c>
     </row>
-    <row r="931" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="931" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A931" s="1" t="s">
         <v>898</v>
       </c>
@@ -42035,7 +42202,7 @@
         <v>3131</v>
       </c>
     </row>
-    <row r="932" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="932" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A932" s="1" t="s">
         <v>899</v>
       </c>
@@ -42046,7 +42213,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="933" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="933" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A933" s="1" t="s">
         <v>900</v>
       </c>
@@ -42057,7 +42224,7 @@
         <v>3133</v>
       </c>
     </row>
-    <row r="934" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="934" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A934" s="1" t="s">
         <v>901</v>
       </c>
@@ -42068,7 +42235,7 @@
         <v>3134</v>
       </c>
     </row>
-    <row r="935" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="935" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A935" s="1" t="s">
         <v>902</v>
       </c>
@@ -42076,10 +42243,19 @@
         <v>3135</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>3135</v>
-      </c>
-    </row>
-    <row r="936" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+        <v>4842</v>
+      </c>
+      <c r="D935" t="b">
+        <v>1</v>
+      </c>
+      <c r="E935" s="1" t="s">
+        <v>4832</v>
+      </c>
+      <c r="F935" s="1" t="s">
+        <v>4843</v>
+      </c>
+    </row>
+    <row r="936" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A936" s="1" t="s">
         <v>903</v>
       </c>
@@ -42090,7 +42266,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="937" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+    <row r="937" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A937" s="1" t="s">
         <v>904</v>
       </c>
@@ -42101,7 +42277,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="938" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="938" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A938" s="1" t="s">
         <v>905</v>
       </c>
@@ -42112,7 +42288,7 @@
         <v>3138</v>
       </c>
     </row>
-    <row r="939" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="939" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A939" s="1" t="s">
         <v>906</v>
       </c>
@@ -42123,7 +42299,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="940" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="940" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A940" s="1" t="s">
         <v>907</v>
       </c>
@@ -42134,7 +42310,7 @@
         <v>3140</v>
       </c>
     </row>
-    <row r="941" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="941" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A941" s="1" t="s">
         <v>908</v>
       </c>
@@ -42145,7 +42321,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="942" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="942" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A942" s="1" t="s">
         <v>909</v>
       </c>
@@ -42156,7 +42332,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="943" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="943" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A943" s="1" t="s">
         <v>910</v>
       </c>
@@ -42167,7 +42343,7 @@
         <v>3143</v>
       </c>
     </row>
-    <row r="944" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="944" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A944" s="1" t="s">
         <v>911</v>
       </c>

</xml_diff>

<commit_message>
[NUS SMS] more labeled data esp for leh51
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
+++ b/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D91A9BA-76A9-4A4A-87AD-CDBC6EB7BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0083D0C4-BF1E-3C41-9F43-F1A3DA0706C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7188" uniqueCount="4844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7148" uniqueCount="4839">
   <si>
     <t>original_sentence</t>
   </si>
@@ -28634,9 +28634,6 @@
 A: You know no matter how many blanks you leave, you probably won't fail right?</t>
   </si>
   <si>
-    <t>["lah21", "lah51"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey, have you checked in at the hotel yet?
 B: Not yet, I was waiting for you.
@@ -28720,9 +28717,6 @@
     <t>delete unimpt cnotext</t>
   </si>
   <si>
-    <t>"lah21"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Hey, you want to come for our morning run
 B: Join lor, since I am up already
@@ -28808,19 +28802,10 @@
     <t>["leh33", "lah24"]</t>
   </si>
   <si>
-    <t>["lah51", "leh33"]</t>
-  </si>
-  <si>
-    <t>["lor33", "leh33"}</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Mei, what do you want to eat for dinner tonight?
 B: Don’t know leh
 A: Everyday don’t know leh don’t know leh, you go out eat yourself lah</t>
-  </si>
-  <si>
-    <t>["leh33", "leh51", "leh51", "lah51"]</t>
   </si>
   <si>
     <t>balance dataset, edit to fit leh51</t>
@@ -29303,8 +29288,8 @@
   <dimension ref="A1:H2245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A934" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B936" sqref="B936"/>
+      <pane ySplit="1" topLeftCell="A809" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F809" sqref="F809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29647,7 +29632,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.2">
@@ -29670,7 +29655,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -29739,7 +29724,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -29785,7 +29770,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30184,7 +30169,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>4804</v>
+        <v>4802</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -30252,7 +30237,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="176" x14ac:dyDescent="0.2">
@@ -30319,7 +30304,7 @@
         <v>2</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>4811</v>
+        <v>4809</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30386,7 +30371,7 @@
         <v>2</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>4812</v>
+        <v>4810</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30442,7 +30427,7 @@
         <v>2</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>4806</v>
+        <v>4804</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30543,7 +30528,7 @@
         <v>2</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>4807</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30566,7 +30551,7 @@
         <v>3</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>4813</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30733,7 +30718,7 @@
         <v>2</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>4807</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -30800,7 +30785,7 @@
         <v>1</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30834,7 +30819,7 @@
         <v>2</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>4808</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -30912,7 +30897,7 @@
         <v>1</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -31246,7 +31231,7 @@
         <v>3</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>4814</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -31522,7 +31507,7 @@
         <v>2</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>4808</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -31783,7 +31768,7 @@
         <v>2</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>4815</v>
+        <v>4813</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -31955,7 +31940,7 @@
         <v>1</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -32045,7 +32030,7 @@
         <v>2</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>4808</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32301,7 +32286,7 @@
         <v>1</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -32393,7 +32378,7 @@
         <v>1</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33246,7 +33231,7 @@
         <v>2</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>4809</v>
+        <v>4807</v>
       </c>
     </row>
     <row r="252" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33269,7 +33254,7 @@
         <v>2</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>4808</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="253" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33292,7 +33277,7 @@
         <v>1</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="254" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -33453,7 +33438,7 @@
         <v>2</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>4815</v>
+        <v>4813</v>
       </c>
     </row>
     <row r="261" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33545,7 +33530,7 @@
         <v>2</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>4809</v>
+        <v>4807</v>
       </c>
     </row>
     <row r="265" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33614,7 +33599,7 @@
         <v>2</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>4806</v>
+        <v>4804</v>
       </c>
     </row>
     <row r="268" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -33660,7 +33645,7 @@
         <v>2</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>4812</v>
+        <v>4810</v>
       </c>
     </row>
     <row r="270" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -33706,7 +33691,7 @@
         <v>4</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>4816</v>
+        <v>4814</v>
       </c>
     </row>
     <row r="272" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -33819,7 +33804,7 @@
         <v>3</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>4817</v>
+        <v>4815</v>
       </c>
     </row>
     <row r="279" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -33897,7 +33882,7 @@
         <v>2</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>4818</v>
+        <v>4816</v>
       </c>
     </row>
     <row r="285" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -33977,7 +33962,7 @@
         <v>3</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>4819</v>
+        <v>4817</v>
       </c>
     </row>
     <row r="289" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -34281,7 +34266,7 @@
         <v>2</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>4818</v>
+        <v>4816</v>
       </c>
     </row>
     <row r="309" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34326,7 +34311,7 @@
         <v>2</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>4815</v>
+        <v>4813</v>
       </c>
     </row>
     <row r="312" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -34851,7 +34836,7 @@
         <v>3</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>4820</v>
+        <v>4818</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -34874,7 +34859,7 @@
         <v>2</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>4821</v>
+        <v>4819</v>
       </c>
     </row>
     <row r="352" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -34897,7 +34882,7 @@
         <v>2</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>4810</v>
+        <v>4808</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -34943,7 +34928,7 @@
         <v>3</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>4822</v>
+        <v>4820</v>
       </c>
     </row>
     <row r="355" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -34983,7 +34968,7 @@
         <v>1</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35006,7 +34991,7 @@
         <v>2</v>
       </c>
       <c r="G357" s="1" t="s">
-        <v>4823</v>
+        <v>4821</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35029,7 +35014,7 @@
         <v>2</v>
       </c>
       <c r="G358" s="1" t="s">
-        <v>4824</v>
+        <v>4822</v>
       </c>
     </row>
     <row r="359" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35138,7 +35123,7 @@
         <v>2</v>
       </c>
       <c r="G363" s="1" t="s">
-        <v>4812</v>
+        <v>4810</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -35221,7 +35206,7 @@
         <v>3</v>
       </c>
       <c r="G367" s="1" t="s">
-        <v>4825</v>
+        <v>4823</v>
       </c>
     </row>
     <row r="368" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35244,7 +35229,7 @@
         <v>1</v>
       </c>
       <c r="G368" s="1" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="369" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35368,7 +35353,7 @@
         <v>3</v>
       </c>
       <c r="G376" s="1" t="s">
-        <v>4826</v>
+        <v>4824</v>
       </c>
     </row>
     <row r="377" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -35675,7 +35660,7 @@
         <v>2</v>
       </c>
       <c r="G399" s="1" t="s">
-        <v>4827</v>
+        <v>4825</v>
       </c>
     </row>
     <row r="400" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35750,7 +35735,10 @@
       <c r="E404" s="1" t="s">
         <v>4736</v>
       </c>
-      <c r="F404" s="1" t="s">
+      <c r="F404">
+        <v>2</v>
+      </c>
+      <c r="G404" s="1" t="s">
         <v>4586</v>
       </c>
     </row>
@@ -35770,8 +35758,11 @@
       <c r="E405" s="1" t="s">
         <v>4738</v>
       </c>
-      <c r="F405" s="1" t="s">
-        <v>4818</v>
+      <c r="F405">
+        <v>2</v>
+      </c>
+      <c r="G405" s="1" t="s">
+        <v>4816</v>
       </c>
     </row>
     <row r="406" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -35801,8 +35792,11 @@
       <c r="E407" s="1" t="s">
         <v>4740</v>
       </c>
-      <c r="F407" s="1" t="s">
-        <v>4805</v>
+      <c r="F407">
+        <v>1</v>
+      </c>
+      <c r="G407" s="1" t="s">
+        <v>4803</v>
       </c>
     </row>
     <row r="408" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -35821,7 +35815,10 @@
       <c r="E408" s="1" t="s">
         <v>4742</v>
       </c>
-      <c r="F408" s="1" t="s">
+      <c r="F408">
+        <v>1</v>
+      </c>
+      <c r="G408" s="1" t="s">
         <v>4578</v>
       </c>
     </row>
@@ -35841,7 +35838,10 @@
       <c r="E409" s="1" t="s">
         <v>4744</v>
       </c>
-      <c r="F409" s="1" t="s">
+      <c r="F409">
+        <v>2</v>
+      </c>
+      <c r="G409" s="1" t="s">
         <v>4586</v>
       </c>
     </row>
@@ -35872,7 +35872,10 @@
       <c r="E411" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F411" s="1" t="s">
+      <c r="F411">
+        <v>2</v>
+      </c>
+      <c r="G411" s="1" t="s">
         <v>4585</v>
       </c>
     </row>
@@ -35914,11 +35917,8 @@
       <c r="E414" s="1" t="s">
         <v>4747</v>
       </c>
-      <c r="F414">
+      <c r="G414">
         <v>2</v>
-      </c>
-      <c r="G414" s="1" t="s">
-        <v>4828</v>
       </c>
     </row>
     <row r="415" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -35937,11 +35937,8 @@
       <c r="E415" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F415" s="1">
+      <c r="G415" s="1">
         <v>1</v>
-      </c>
-      <c r="G415" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="416" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35960,11 +35957,8 @@
       <c r="E416" s="1" t="s">
         <v>4750</v>
       </c>
-      <c r="F416">
+      <c r="G416">
         <v>1</v>
-      </c>
-      <c r="G416" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="417" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36055,11 +36049,8 @@
       <c r="E423" s="1" t="s">
         <v>4753</v>
       </c>
-      <c r="F423">
+      <c r="G423">
         <v>2</v>
-      </c>
-      <c r="G423" s="1" t="s">
-        <v>4811</v>
       </c>
     </row>
     <row r="424" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -36122,11 +36113,8 @@
       <c r="E428" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F428">
+      <c r="G428">
         <v>1</v>
-      </c>
-      <c r="G428" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="429" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36145,11 +36133,8 @@
       <c r="E429" s="1" t="s">
         <v>4628</v>
       </c>
-      <c r="F429">
+      <c r="G429">
         <v>2</v>
-      </c>
-      <c r="G429" s="1" t="s">
-        <v>4821</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -36207,11 +36192,8 @@
       <c r="E433" s="1" t="s">
         <v>4758</v>
       </c>
-      <c r="F433">
+      <c r="G433">
         <v>1</v>
-      </c>
-      <c r="G433" s="1" t="s">
-        <v>4578</v>
       </c>
     </row>
     <row r="434" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36252,11 +36234,8 @@
       <c r="E436" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="F436">
+      <c r="G436">
         <v>1</v>
-      </c>
-      <c r="G436" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="437" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36286,11 +36265,8 @@
       <c r="E438" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F438" s="1">
+      <c r="G438" s="1">
         <v>1</v>
-      </c>
-      <c r="G438" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="439" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36309,11 +36285,8 @@
       <c r="E439" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="F439">
+      <c r="G439">
         <v>1</v>
-      </c>
-      <c r="G439" s="1" t="s">
-        <v>4578</v>
       </c>
     </row>
     <row r="440" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36376,11 +36349,8 @@
       <c r="E444" s="1" t="s">
         <v>4639</v>
       </c>
-      <c r="F444">
+      <c r="G444">
         <v>1</v>
-      </c>
-      <c r="G444" s="1" t="s">
-        <v>4805</v>
       </c>
     </row>
     <row r="445" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36399,11 +36369,8 @@
       <c r="E445" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="F445" s="1">
+      <c r="G445" s="1">
         <v>1</v>
-      </c>
-      <c r="G445" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="446" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36444,11 +36411,8 @@
       <c r="E448" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F448" s="1">
+      <c r="G448" s="1">
         <v>1</v>
-      </c>
-      <c r="G448" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="449" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -36478,11 +36442,8 @@
       <c r="E450" s="1" t="s">
         <v>4766</v>
       </c>
-      <c r="F450">
+      <c r="G450">
         <v>1</v>
-      </c>
-      <c r="G450" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="451" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36617,11 +36578,8 @@
       <c r="E461" s="1" t="s">
         <v>4769</v>
       </c>
-      <c r="F461">
+      <c r="G461">
         <v>1</v>
-      </c>
-      <c r="G461" s="1" t="s">
-        <v>4804</v>
       </c>
     </row>
     <row r="462" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36816,11 +36774,8 @@
       <c r="E478" s="1" t="s">
         <v>4771</v>
       </c>
-      <c r="F478">
+      <c r="G478">
         <v>1</v>
-      </c>
-      <c r="G478" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="479" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -36872,11 +36827,8 @@
       <c r="E482" s="1" t="s">
         <v>4773</v>
       </c>
-      <c r="F482">
+      <c r="G482">
         <v>1</v>
-      </c>
-      <c r="G482" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="483" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -37111,11 +37063,8 @@
       <c r="E501" s="1" t="s">
         <v>4776</v>
       </c>
-      <c r="F501">
+      <c r="G501">
         <v>2</v>
-      </c>
-      <c r="G501" s="1" t="s">
-        <v>4585</v>
       </c>
     </row>
     <row r="502" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37173,11 +37122,8 @@
       <c r="E505" s="1" t="s">
         <v>4639</v>
       </c>
-      <c r="F505">
+      <c r="G505">
         <v>1</v>
-      </c>
-      <c r="G505" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="506" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37207,11 +37153,8 @@
       <c r="E507" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F507">
+      <c r="G507">
         <v>1</v>
-      </c>
-      <c r="G507" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="508" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37252,11 +37195,8 @@
       <c r="E510" s="1" t="s">
         <v>4742</v>
       </c>
-      <c r="F510">
+      <c r="G510">
         <v>1</v>
-      </c>
-      <c r="G510" s="1" t="s">
-        <v>4587</v>
       </c>
     </row>
     <row r="511" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37275,11 +37215,8 @@
       <c r="E511" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F511">
+      <c r="G511">
         <v>1</v>
-      </c>
-      <c r="G511" s="1" t="s">
-        <v>4584</v>
       </c>
     </row>
     <row r="512" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37298,11 +37235,8 @@
       <c r="E512" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F512">
+      <c r="G512">
         <v>1</v>
-      </c>
-      <c r="G512" s="1" t="s">
-        <v>4578</v>
       </c>
     </row>
     <row r="513" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37401,7 +37335,7 @@
         <v>2721</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>4803</v>
+        <v>4801</v>
       </c>
       <c r="D521" t="b">
         <v>1</v>
@@ -37409,11 +37343,8 @@
       <c r="E521" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F521">
+      <c r="G521">
         <v>2</v>
-      </c>
-      <c r="G521" s="1" t="s">
-        <v>4821</v>
       </c>
     </row>
     <row r="522" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37454,11 +37385,8 @@
       <c r="E524" s="1" t="s">
         <v>4783</v>
       </c>
-      <c r="F524">
+      <c r="G524">
         <v>1</v>
-      </c>
-      <c r="G524" s="1" t="s">
-        <v>4805</v>
       </c>
     </row>
     <row r="525" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37519,7 +37447,7 @@
         <v>2729</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>4802</v>
+        <v>4800</v>
       </c>
       <c r="D529" t="b">
         <v>1</v>
@@ -37527,11 +37455,8 @@
       <c r="E529" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="F529">
+      <c r="G529">
         <v>1</v>
-      </c>
-      <c r="G529" s="1" t="s">
-        <v>4578</v>
       </c>
     </row>
     <row r="530" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37553,19 +37478,16 @@
         <v>2731</v>
       </c>
       <c r="C531" s="1" t="s">
-        <v>4799</v>
+        <v>4798</v>
       </c>
       <c r="D531" t="b">
         <v>1</v>
       </c>
       <c r="E531" s="1" t="s">
-        <v>4800</v>
-      </c>
-      <c r="F531" s="1">
+        <v>4799</v>
+      </c>
+      <c r="G531" s="1">
         <v>1</v>
-      </c>
-      <c r="G531" s="1" t="s">
-        <v>4801</v>
       </c>
     </row>
     <row r="532" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37595,11 +37517,8 @@
       <c r="E533" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F533">
+      <c r="G533">
         <v>2</v>
-      </c>
-      <c r="G533" s="1" t="s">
-        <v>4785</v>
       </c>
     </row>
     <row r="534" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37621,19 +37540,16 @@
         <v>2735</v>
       </c>
       <c r="C535" s="1" t="s">
-        <v>4786</v>
+        <v>4785</v>
       </c>
       <c r="D535" t="b">
         <v>1</v>
       </c>
       <c r="E535" s="1" t="s">
-        <v>4787</v>
-      </c>
-      <c r="F535">
+        <v>4786</v>
+      </c>
+      <c r="G535">
         <v>1</v>
-      </c>
-      <c r="G535" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="536" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37655,19 +37571,16 @@
         <v>2737</v>
       </c>
       <c r="C537" s="1" t="s">
-        <v>4788</v>
+        <v>4787</v>
       </c>
       <c r="D537" t="b">
         <v>1</v>
       </c>
       <c r="E537" s="1" t="s">
-        <v>4787</v>
-      </c>
-      <c r="F537">
+        <v>4786</v>
+      </c>
+      <c r="G537">
         <v>1</v>
-      </c>
-      <c r="G537" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="538" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37689,19 +37602,16 @@
         <v>2739</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>4789</v>
+        <v>4788</v>
       </c>
       <c r="D539" t="b">
         <v>1</v>
       </c>
       <c r="E539" s="1" t="s">
-        <v>4787</v>
-      </c>
-      <c r="F539">
+        <v>4786</v>
+      </c>
+      <c r="G539">
         <v>1</v>
-      </c>
-      <c r="G539" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="540" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37723,19 +37633,16 @@
         <v>2741</v>
       </c>
       <c r="C541" s="1" t="s">
-        <v>4790</v>
+        <v>4789</v>
       </c>
       <c r="D541" t="b">
         <v>1</v>
       </c>
       <c r="E541" s="1" t="s">
-        <v>4787</v>
-      </c>
-      <c r="F541">
+        <v>4786</v>
+      </c>
+      <c r="G541">
         <v>1</v>
-      </c>
-      <c r="G541" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="542" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -37746,7 +37653,7 @@
         <v>2742</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>4791</v>
+        <v>4790</v>
       </c>
       <c r="D542" t="b">
         <v>1</v>
@@ -37754,11 +37661,8 @@
       <c r="E542" s="1" t="s">
         <v>4535</v>
       </c>
-      <c r="F542">
+      <c r="G542">
         <v>2</v>
-      </c>
-      <c r="G542" s="1" t="s">
-        <v>4829</v>
       </c>
     </row>
     <row r="543" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37780,7 +37684,7 @@
         <v>2744</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>4792</v>
+        <v>4791</v>
       </c>
       <c r="D544" t="b">
         <v>1</v>
@@ -37788,11 +37692,8 @@
       <c r="E544" s="1" t="s">
         <v>4639</v>
       </c>
-      <c r="F544">
+      <c r="G544">
         <v>1</v>
-      </c>
-      <c r="G544" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37803,19 +37704,16 @@
         <v>2745</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>4793</v>
+        <v>4792</v>
       </c>
       <c r="D545" t="b">
         <v>1</v>
       </c>
       <c r="E545" s="1" t="s">
-        <v>4794</v>
-      </c>
-      <c r="F545">
+        <v>4793</v>
+      </c>
+      <c r="G545">
         <v>2</v>
-      </c>
-      <c r="G545" s="1" t="s">
-        <v>4807</v>
       </c>
     </row>
     <row r="546" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37826,7 +37724,7 @@
         <v>2746</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="D546" t="b">
         <v>1</v>
@@ -37834,11 +37732,8 @@
       <c r="E546" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F546">
+      <c r="G546">
         <v>1</v>
-      </c>
-      <c r="G546" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="547" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37849,19 +37744,16 @@
         <v>2747</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>4796</v>
+        <v>4795</v>
       </c>
       <c r="D547" t="b">
         <v>1</v>
       </c>
       <c r="E547" s="1" t="s">
-        <v>4787</v>
-      </c>
-      <c r="F547">
+        <v>4786</v>
+      </c>
+      <c r="G547">
         <v>2</v>
-      </c>
-      <c r="G547" s="1" t="s">
-        <v>4815</v>
       </c>
     </row>
     <row r="548" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -37872,7 +37764,7 @@
         <v>2748</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>4797</v>
+        <v>4796</v>
       </c>
       <c r="D548" t="b">
         <v>1</v>
@@ -37880,11 +37772,8 @@
       <c r="E548" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="F548">
+      <c r="G548">
         <v>1</v>
-      </c>
-      <c r="G548" s="1" t="s">
-        <v>4580</v>
       </c>
     </row>
     <row r="549" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37895,7 +37784,7 @@
         <v>2749</v>
       </c>
       <c r="C549" s="1" t="s">
-        <v>4798</v>
+        <v>4797</v>
       </c>
       <c r="D549" t="b">
         <v>1</v>
@@ -37903,11 +37792,8 @@
       <c r="E549" s="1" t="s">
         <v>4497</v>
       </c>
-      <c r="F549">
+      <c r="G549">
         <v>1</v>
-      </c>
-      <c r="G549" s="1" t="s">
-        <v>4583</v>
       </c>
     </row>
     <row r="550" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -38705,19 +38591,16 @@
         <v>2821</v>
       </c>
       <c r="C621" s="1" t="s">
-        <v>4830</v>
+        <v>4826</v>
       </c>
       <c r="D621" t="b">
         <v>1</v>
       </c>
       <c r="E621" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F621">
+        <v>4827</v>
+      </c>
+      <c r="G621">
         <v>4</v>
-      </c>
-      <c r="G621" s="1" t="s">
-        <v>4831</v>
       </c>
     </row>
     <row r="622" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -38753,7 +38636,7 @@
         <v>2824</v>
       </c>
     </row>
-    <row r="625" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A625" s="1" t="s">
         <v>598</v>
       </c>
@@ -38764,7 +38647,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="626" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A626" s="1" t="s">
         <v>599</v>
       </c>
@@ -38772,19 +38655,22 @@
         <v>2826</v>
       </c>
       <c r="C626" s="1" t="s">
-        <v>4833</v>
+        <v>4828</v>
       </c>
       <c r="D626" t="b">
         <v>1</v>
       </c>
       <c r="E626" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F626" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="627" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F626">
+        <v>1</v>
+      </c>
+      <c r="G626" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="627" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A627" s="1" t="s">
         <v>600</v>
       </c>
@@ -38795,7 +38681,7 @@
         <v>2827</v>
       </c>
     </row>
-    <row r="628" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A628" s="1" t="s">
         <v>601</v>
       </c>
@@ -38806,7 +38692,7 @@
         <v>2828</v>
       </c>
     </row>
-    <row r="629" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A629" s="1" t="s">
         <v>602</v>
       </c>
@@ -38817,7 +38703,7 @@
         <v>2829</v>
       </c>
     </row>
-    <row r="630" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A630" s="1" t="s">
         <v>603</v>
       </c>
@@ -38828,7 +38714,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="631" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A631" s="1" t="s">
         <v>604</v>
       </c>
@@ -38839,7 +38725,7 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="632" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="632" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A632" s="1" t="s">
         <v>605</v>
       </c>
@@ -38850,7 +38736,7 @@
         <v>2832</v>
       </c>
     </row>
-    <row r="633" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="633" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A633" s="1" t="s">
         <v>606</v>
       </c>
@@ -38861,7 +38747,7 @@
         <v>2833</v>
       </c>
     </row>
-    <row r="634" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A634" s="1" t="s">
         <v>607</v>
       </c>
@@ -38872,7 +38758,7 @@
         <v>2834</v>
       </c>
     </row>
-    <row r="635" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A635" s="1" t="s">
         <v>608</v>
       </c>
@@ -38883,7 +38769,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="636" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A636" s="1" t="s">
         <v>609</v>
       </c>
@@ -38894,7 +38780,7 @@
         <v>2836</v>
       </c>
     </row>
-    <row r="637" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A637" s="1" t="s">
         <v>610</v>
       </c>
@@ -38905,7 +38791,7 @@
         <v>2837</v>
       </c>
     </row>
-    <row r="638" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A638" s="1" t="s">
         <v>611</v>
       </c>
@@ -38916,7 +38802,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="639" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A639" s="1" t="s">
         <v>612</v>
       </c>
@@ -38927,7 +38813,7 @@
         <v>2839</v>
       </c>
     </row>
-    <row r="640" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A640" s="1" t="s">
         <v>613</v>
       </c>
@@ -39290,7 +39176,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="673" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="673" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A673" s="1" t="s">
         <v>646</v>
       </c>
@@ -39301,7 +39187,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="674" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="674" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A674" s="1" t="s">
         <v>647</v>
       </c>
@@ -39312,7 +39198,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="675" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="675" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A675" s="1" t="s">
         <v>648</v>
       </c>
@@ -39323,7 +39209,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="676" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A676" s="1" t="s">
         <v>649</v>
       </c>
@@ -39334,7 +39220,7 @@
         <v>2876</v>
       </c>
     </row>
-    <row r="677" spans="1:6" ht="192" x14ac:dyDescent="0.2">
+    <row r="677" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A677" s="1" t="s">
         <v>650</v>
       </c>
@@ -39342,19 +39228,22 @@
         <v>2877</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>4834</v>
+        <v>4829</v>
       </c>
       <c r="D677" t="b">
         <v>1</v>
       </c>
       <c r="E677" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F677" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="678" spans="1:6" ht="208" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F677">
+        <v>1</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="678" spans="1:7" ht="208" x14ac:dyDescent="0.2">
       <c r="A678" s="1" t="s">
         <v>651</v>
       </c>
@@ -39365,7 +39254,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="679" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="679" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A679" s="1" t="s">
         <v>652</v>
       </c>
@@ -39376,7 +39265,7 @@
         <v>2879</v>
       </c>
     </row>
-    <row r="680" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="680" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A680" s="1" t="s">
         <v>653</v>
       </c>
@@ -39387,7 +39276,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="681" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="681" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A681" s="1" t="s">
         <v>654</v>
       </c>
@@ -39398,7 +39287,7 @@
         <v>2881</v>
       </c>
     </row>
-    <row r="682" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="682" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A682" s="1" t="s">
         <v>655</v>
       </c>
@@ -39409,7 +39298,7 @@
         <v>2882</v>
       </c>
     </row>
-    <row r="683" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="683" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A683" s="1" t="s">
         <v>656</v>
       </c>
@@ -39420,7 +39309,7 @@
         <v>2883</v>
       </c>
     </row>
-    <row r="684" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="684" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A684" s="1" t="s">
         <v>657</v>
       </c>
@@ -39431,7 +39320,7 @@
         <v>2884</v>
       </c>
     </row>
-    <row r="685" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="685" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A685" s="1" t="s">
         <v>658</v>
       </c>
@@ -39442,7 +39331,7 @@
         <v>2885</v>
       </c>
     </row>
-    <row r="686" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A686" s="1" t="s">
         <v>659</v>
       </c>
@@ -39453,7 +39342,7 @@
         <v>2886</v>
       </c>
     </row>
-    <row r="687" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A687" s="1" t="s">
         <v>660</v>
       </c>
@@ -39464,7 +39353,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="688" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A688" s="1" t="s">
         <v>661</v>
       </c>
@@ -39827,7 +39716,7 @@
         <v>2920</v>
       </c>
     </row>
-    <row r="721" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="721" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A721" s="1" t="s">
         <v>694</v>
       </c>
@@ -39838,7 +39727,7 @@
         <v>2921</v>
       </c>
     </row>
-    <row r="722" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="722" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A722" s="1" t="s">
         <v>695</v>
       </c>
@@ -39849,7 +39738,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="723" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="723" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A723" s="1" t="s">
         <v>696</v>
       </c>
@@ -39860,7 +39749,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="724" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="724" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A724" s="1" t="s">
         <v>697</v>
       </c>
@@ -39871,7 +39760,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="725" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="725" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A725" s="1" t="s">
         <v>698</v>
       </c>
@@ -39882,7 +39771,7 @@
         <v>2925</v>
       </c>
     </row>
-    <row r="726" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="726" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A726" s="1" t="s">
         <v>699</v>
       </c>
@@ -39893,7 +39782,7 @@
         <v>2926</v>
       </c>
     </row>
-    <row r="727" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="727" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A727" s="1" t="s">
         <v>700</v>
       </c>
@@ -39904,7 +39793,7 @@
         <v>2927</v>
       </c>
     </row>
-    <row r="728" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="728" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A728" s="1" t="s">
         <v>701</v>
       </c>
@@ -39915,7 +39804,7 @@
         <v>2928</v>
       </c>
     </row>
-    <row r="729" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A729" s="1" t="s">
         <v>702</v>
       </c>
@@ -39926,7 +39815,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="730" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="730" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A730" s="1" t="s">
         <v>703</v>
       </c>
@@ -39937,7 +39826,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="731" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="731" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A731" s="1" t="s">
         <v>704</v>
       </c>
@@ -39945,19 +39834,22 @@
         <v>2931</v>
       </c>
       <c r="C731" s="1" t="s">
-        <v>4835</v>
+        <v>4830</v>
       </c>
       <c r="D731" t="b">
         <v>1</v>
       </c>
       <c r="E731" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F731" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="732" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F731">
+        <v>1</v>
+      </c>
+      <c r="G731" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="732" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A732" s="1" t="s">
         <v>705</v>
       </c>
@@ -39968,7 +39860,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="733" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="733" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A733" s="1" t="s">
         <v>706</v>
       </c>
@@ -39979,7 +39871,7 @@
         <v>2933</v>
       </c>
     </row>
-    <row r="734" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="734" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A734" s="1" t="s">
         <v>707</v>
       </c>
@@ -39990,7 +39882,7 @@
         <v>2934</v>
       </c>
     </row>
-    <row r="735" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="735" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A735" s="1" t="s">
         <v>708</v>
       </c>
@@ -39998,19 +39890,22 @@
         <v>2935</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>4836</v>
+        <v>4831</v>
       </c>
       <c r="D735" t="b">
         <v>1</v>
       </c>
       <c r="E735" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F735" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="736" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F735">
+        <v>1</v>
+      </c>
+      <c r="G735" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="736" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A736" s="1" t="s">
         <v>709</v>
       </c>
@@ -40197,7 +40092,7 @@
         <v>2952</v>
       </c>
     </row>
-    <row r="753" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A753" s="1" t="s">
         <v>725</v>
       </c>
@@ -40208,7 +40103,7 @@
         <v>2953</v>
       </c>
     </row>
-    <row r="754" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="754" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A754" s="1" t="s">
         <v>726</v>
       </c>
@@ -40219,7 +40114,7 @@
         <v>2954</v>
       </c>
     </row>
-    <row r="755" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="755" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A755" s="1" t="s">
         <v>727</v>
       </c>
@@ -40230,7 +40125,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="756" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="756" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A756" s="1" t="s">
         <v>728</v>
       </c>
@@ -40241,7 +40136,7 @@
         <v>2956</v>
       </c>
     </row>
-    <row r="757" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="757" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A757" s="1" t="s">
         <v>729</v>
       </c>
@@ -40252,7 +40147,7 @@
         <v>2957</v>
       </c>
     </row>
-    <row r="758" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="758" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A758" s="1" t="s">
         <v>730</v>
       </c>
@@ -40263,7 +40158,7 @@
         <v>2958</v>
       </c>
     </row>
-    <row r="759" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="759" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A759" s="1" t="s">
         <v>731</v>
       </c>
@@ -40271,19 +40166,22 @@
         <v>2959</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>4837</v>
+        <v>4832</v>
       </c>
       <c r="D759" t="b">
         <v>1</v>
       </c>
       <c r="E759" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F759" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="760" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F759">
+        <v>1</v>
+      </c>
+      <c r="G759" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="760" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A760" s="1" t="s">
         <v>732</v>
       </c>
@@ -40294,7 +40192,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="761" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A761" s="1" t="s">
         <v>733</v>
       </c>
@@ -40305,7 +40203,7 @@
         <v>2961</v>
       </c>
     </row>
-    <row r="762" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="762" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A762" s="1" t="s">
         <v>734</v>
       </c>
@@ -40316,7 +40214,7 @@
         <v>2962</v>
       </c>
     </row>
-    <row r="763" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="763" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A763" s="1" t="s">
         <v>735</v>
       </c>
@@ -40327,7 +40225,7 @@
         <v>2963</v>
       </c>
     </row>
-    <row r="764" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="764" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A764" s="1" t="s">
         <v>736</v>
       </c>
@@ -40338,7 +40236,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="765" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="765" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A765" s="1" t="s">
         <v>737</v>
       </c>
@@ -40349,7 +40247,7 @@
         <v>2965</v>
       </c>
     </row>
-    <row r="766" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="766" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A766" s="1" t="s">
         <v>738</v>
       </c>
@@ -40360,7 +40258,7 @@
         <v>2966</v>
       </c>
     </row>
-    <row r="767" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="767" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A767" s="1" t="s">
         <v>739</v>
       </c>
@@ -40371,7 +40269,7 @@
         <v>2967</v>
       </c>
     </row>
-    <row r="768" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A768" s="1" t="s">
         <v>740</v>
       </c>
@@ -40379,7 +40277,7 @@
         <v>2968</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>4838</v>
+        <v>4833</v>
       </c>
     </row>
     <row r="769" spans="1:3" ht="128" x14ac:dyDescent="0.2">
@@ -40734,7 +40632,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="801" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="801" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A801" s="1" t="s">
         <v>773</v>
       </c>
@@ -40745,7 +40643,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="802" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A802" s="1" t="s">
         <v>774</v>
       </c>
@@ -40756,7 +40654,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="803" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="803" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A803" s="1" t="s">
         <v>775</v>
       </c>
@@ -40767,7 +40665,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="804" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A804" s="1" t="s">
         <v>776</v>
       </c>
@@ -40778,7 +40676,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="805" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="805" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A805" s="1" t="s">
         <v>777</v>
       </c>
@@ -40789,7 +40687,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row r="806" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="806" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A806" s="1" t="s">
         <v>778</v>
       </c>
@@ -40800,7 +40698,7 @@
         <v>3006</v>
       </c>
     </row>
-    <row r="807" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="807" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A807" s="1" t="s">
         <v>779</v>
       </c>
@@ -40811,7 +40709,7 @@
         <v>3007</v>
       </c>
     </row>
-    <row r="808" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="808" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A808" s="1" t="s">
         <v>780</v>
       </c>
@@ -40822,7 +40720,7 @@
         <v>3008</v>
       </c>
     </row>
-    <row r="809" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="809" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A809" s="1" t="s">
         <v>781</v>
       </c>
@@ -40830,19 +40728,22 @@
         <v>3009</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>4839</v>
+        <v>4834</v>
       </c>
       <c r="D809" t="b">
         <v>1</v>
       </c>
       <c r="E809" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F809" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="810" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F809">
+        <v>1</v>
+      </c>
+      <c r="G809" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="810" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A810" s="1" t="s">
         <v>782</v>
       </c>
@@ -40853,7 +40754,7 @@
         <v>3010</v>
       </c>
     </row>
-    <row r="811" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="811" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A811" s="1" t="s">
         <v>783</v>
       </c>
@@ -40861,19 +40762,22 @@
         <v>3011</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>4840</v>
+        <v>4835</v>
       </c>
       <c r="D811" t="b">
         <v>1</v>
       </c>
       <c r="E811" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F811" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="812" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F811">
+        <v>1</v>
+      </c>
+      <c r="G811" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="812" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A812" s="1" t="s">
         <v>784</v>
       </c>
@@ -40884,7 +40788,7 @@
         <v>3012</v>
       </c>
     </row>
-    <row r="813" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="813" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A813" s="1" t="s">
         <v>785</v>
       </c>
@@ -40895,7 +40799,7 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="814" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A814" s="1" t="s">
         <v>786</v>
       </c>
@@ -40906,7 +40810,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="815" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="815" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A815" s="1" t="s">
         <v>787</v>
       </c>
@@ -40917,7 +40821,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="816" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="816" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A816" s="1" t="s">
         <v>788</v>
       </c>
@@ -41456,7 +41360,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="865" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A865" s="1" t="s">
         <v>835</v>
       </c>
@@ -41467,7 +41371,7 @@
         <v>3065</v>
       </c>
     </row>
-    <row r="866" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="866" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A866" s="1" t="s">
         <v>836</v>
       </c>
@@ -41478,7 +41382,7 @@
         <v>3066</v>
       </c>
     </row>
-    <row r="867" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="867" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A867" s="1" t="s">
         <v>647</v>
       </c>
@@ -41489,7 +41393,7 @@
         <v>3067</v>
       </c>
     </row>
-    <row r="868" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="868" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A868" s="1" t="s">
         <v>837</v>
       </c>
@@ -41500,7 +41404,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="869" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="869" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A869" s="1" t="s">
         <v>838</v>
       </c>
@@ -41511,7 +41415,7 @@
         <v>3069</v>
       </c>
     </row>
-    <row r="870" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="870" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A870" s="1" t="s">
         <v>839</v>
       </c>
@@ -41522,7 +41426,7 @@
         <v>3070</v>
       </c>
     </row>
-    <row r="871" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="871" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A871" s="1" t="s">
         <v>840</v>
       </c>
@@ -41533,7 +41437,7 @@
         <v>3071</v>
       </c>
     </row>
-    <row r="872" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="872" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A872" s="1" t="s">
         <v>841</v>
       </c>
@@ -41544,7 +41448,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="873" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="873" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A873" s="1" t="s">
         <v>842</v>
       </c>
@@ -41555,7 +41459,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="874" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="874" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A874" s="1" t="s">
         <v>843</v>
       </c>
@@ -41566,7 +41470,7 @@
         <v>3074</v>
       </c>
     </row>
-    <row r="875" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="875" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A875" s="1" t="s">
         <v>844</v>
       </c>
@@ -41574,19 +41478,22 @@
         <v>3075</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>4841</v>
+        <v>4836</v>
       </c>
       <c r="D875" t="b">
         <v>1</v>
       </c>
       <c r="E875" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F875" s="1" t="s">
-        <v>4804</v>
-      </c>
-    </row>
-    <row r="876" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F875">
+        <v>1</v>
+      </c>
+      <c r="G875" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="876" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A876" s="1" t="s">
         <v>845</v>
       </c>
@@ -41597,7 +41504,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="877" spans="1:6" ht="224" x14ac:dyDescent="0.2">
+    <row r="877" spans="1:7" ht="224" x14ac:dyDescent="0.2">
       <c r="A877" s="1" t="s">
         <v>846</v>
       </c>
@@ -41608,7 +41515,7 @@
         <v>3077</v>
       </c>
     </row>
-    <row r="878" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="878" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A878" s="1" t="s">
         <v>847</v>
       </c>
@@ -41619,7 +41526,7 @@
         <v>3078</v>
       </c>
     </row>
-    <row r="879" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="879" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A879" s="1" t="s">
         <v>848</v>
       </c>
@@ -41630,7 +41537,7 @@
         <v>3079</v>
       </c>
     </row>
-    <row r="880" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="880" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A880" s="1" t="s">
         <v>849</v>
       </c>
@@ -42169,7 +42076,7 @@
         <v>3128</v>
       </c>
     </row>
-    <row r="929" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="929" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A929" s="1" t="s">
         <v>896</v>
       </c>
@@ -42180,7 +42087,7 @@
         <v>3129</v>
       </c>
     </row>
-    <row r="930" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="930" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A930" s="1" t="s">
         <v>897</v>
       </c>
@@ -42191,7 +42098,7 @@
         <v>3130</v>
       </c>
     </row>
-    <row r="931" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="931" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A931" s="1" t="s">
         <v>898</v>
       </c>
@@ -42202,7 +42109,7 @@
         <v>3131</v>
       </c>
     </row>
-    <row r="932" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="932" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A932" s="1" t="s">
         <v>899</v>
       </c>
@@ -42213,7 +42120,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="933" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="933" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A933" s="1" t="s">
         <v>900</v>
       </c>
@@ -42224,7 +42131,7 @@
         <v>3133</v>
       </c>
     </row>
-    <row r="934" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="934" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A934" s="1" t="s">
         <v>901</v>
       </c>
@@ -42235,7 +42142,7 @@
         <v>3134</v>
       </c>
     </row>
-    <row r="935" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="935" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A935" s="1" t="s">
         <v>902</v>
       </c>
@@ -42243,19 +42150,22 @@
         <v>3135</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>4842</v>
+        <v>4837</v>
       </c>
       <c r="D935" t="b">
         <v>1</v>
       </c>
       <c r="E935" s="1" t="s">
-        <v>4832</v>
-      </c>
-      <c r="F935" s="1" t="s">
-        <v>4843</v>
-      </c>
-    </row>
-    <row r="936" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+        <v>4827</v>
+      </c>
+      <c r="F935">
+        <v>2</v>
+      </c>
+      <c r="G935" s="1" t="s">
+        <v>4838</v>
+      </c>
+    </row>
+    <row r="936" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A936" s="1" t="s">
         <v>903</v>
       </c>
@@ -42266,7 +42176,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="937" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="937" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A937" s="1" t="s">
         <v>904</v>
       </c>
@@ -42277,7 +42187,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="938" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="938" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A938" s="1" t="s">
         <v>905</v>
       </c>
@@ -42288,7 +42198,7 @@
         <v>3138</v>
       </c>
     </row>
-    <row r="939" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+    <row r="939" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A939" s="1" t="s">
         <v>906</v>
       </c>
@@ -42299,7 +42209,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="940" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="940" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A940" s="1" t="s">
         <v>907</v>
       </c>
@@ -42310,7 +42220,7 @@
         <v>3140</v>
       </c>
     </row>
-    <row r="941" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="941" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A941" s="1" t="s">
         <v>908</v>
       </c>
@@ -42321,7 +42231,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="942" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="942" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A942" s="1" t="s">
         <v>909</v>
       </c>
@@ -42332,7 +42242,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="943" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="943" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A943" s="1" t="s">
         <v>910</v>
       </c>
@@ -42343,7 +42253,7 @@
         <v>3143</v>
       </c>
     </row>
-    <row r="944" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="944" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A944" s="1" t="s">
         <v>911</v>
       </c>

</xml_diff>

<commit_message>
clean NUS SMS dataset and run script to create final dataset
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
+++ b/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/processed_step_4_manual_label.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/singlish_NUS_SMS/processed_step_4_manual_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0083D0C4-BF1E-3C41-9F43-F1A3DA0706C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C9229D-FBA3-0A4B-90C0-E0CF4EAB1438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7148" uniqueCount="4839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7189" uniqueCount="4842">
   <si>
     <t>original_sentence</t>
   </si>
@@ -28881,12 +28881,21 @@
   <si>
     <t>["leh51", "lah21"]</t>
   </si>
+  <si>
+    <t>["lah51", "leh33"]</t>
+  </si>
+  <si>
+    <t>["lah21", "lah51"]</t>
+  </si>
+  <si>
+    <t>["leh33", "leh51", "leh51", "lah51"]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28908,6 +28917,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -28951,7 +28966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -28967,6 +28982,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -29288,8 +29304,8 @@
   <dimension ref="A1:H2245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A809" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F809" sqref="F809"/>
+      <pane ySplit="1" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E542" sqref="E542"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35917,8 +35933,11 @@
       <c r="E414" s="1" t="s">
         <v>4747</v>
       </c>
-      <c r="G414">
+      <c r="F414" s="7">
         <v>2</v>
+      </c>
+      <c r="G414" s="7" t="s">
+        <v>4839</v>
       </c>
     </row>
     <row r="415" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -35937,8 +35956,11 @@
       <c r="E415" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G415" s="1">
+      <c r="F415" s="7">
         <v>1</v>
+      </c>
+      <c r="G415" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="416" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -35957,8 +35979,11 @@
       <c r="E416" s="1" t="s">
         <v>4750</v>
       </c>
-      <c r="G416">
+      <c r="F416" s="7">
         <v>1</v>
+      </c>
+      <c r="G416" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="417" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36049,8 +36074,11 @@
       <c r="E423" s="1" t="s">
         <v>4753</v>
       </c>
-      <c r="G423">
+      <c r="F423" s="7">
         <v>2</v>
+      </c>
+      <c r="G423" s="7" t="s">
+        <v>4809</v>
       </c>
     </row>
     <row r="424" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -36113,8 +36141,11 @@
       <c r="E428" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G428">
+      <c r="F428" s="7">
         <v>1</v>
+      </c>
+      <c r="G428" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="429" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36133,8 +36164,11 @@
       <c r="E429" s="1" t="s">
         <v>4628</v>
       </c>
-      <c r="G429">
+      <c r="F429" s="7">
         <v>2</v>
+      </c>
+      <c r="G429" s="7" t="s">
+        <v>4819</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -36192,8 +36226,11 @@
       <c r="E433" s="1" t="s">
         <v>4758</v>
       </c>
-      <c r="G433">
+      <c r="F433" s="7">
         <v>1</v>
+      </c>
+      <c r="G433" s="7" t="s">
+        <v>4578</v>
       </c>
     </row>
     <row r="434" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36234,8 +36271,11 @@
       <c r="E436" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="G436">
+      <c r="F436" s="7">
         <v>1</v>
+      </c>
+      <c r="G436" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="437" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36248,6 +36288,12 @@
       <c r="C437" s="1" t="s">
         <v>2637</v>
       </c>
+      <c r="F437" s="7">
+        <v>1</v>
+      </c>
+      <c r="G437" s="7" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="438" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
@@ -36265,8 +36311,11 @@
       <c r="E438" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G438" s="1">
+      <c r="F438" s="7">
         <v>1</v>
+      </c>
+      <c r="G438" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="439" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36285,8 +36334,11 @@
       <c r="E439" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="G439">
+      <c r="F439" s="7">
         <v>1</v>
+      </c>
+      <c r="G439" s="7" t="s">
+        <v>4578</v>
       </c>
     </row>
     <row r="440" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36349,8 +36401,11 @@
       <c r="E444" s="1" t="s">
         <v>4639</v>
       </c>
-      <c r="G444">
+      <c r="F444" s="7">
         <v>1</v>
+      </c>
+      <c r="G444" s="7" t="s">
+        <v>4803</v>
       </c>
     </row>
     <row r="445" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36369,8 +36424,11 @@
       <c r="E445" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="G445" s="1">
+      <c r="F445" s="7">
         <v>1</v>
+      </c>
+      <c r="G445" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="446" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36411,8 +36469,11 @@
       <c r="E448" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G448" s="1">
+      <c r="F448" s="7">
         <v>1</v>
+      </c>
+      <c r="G448" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="449" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -36442,8 +36503,11 @@
       <c r="E450" s="1" t="s">
         <v>4766</v>
       </c>
-      <c r="G450">
+      <c r="F450" s="7">
         <v>1</v>
+      </c>
+      <c r="G450" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="451" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -36578,8 +36642,11 @@
       <c r="E461" s="1" t="s">
         <v>4769</v>
       </c>
-      <c r="G461">
+      <c r="F461" s="7">
         <v>1</v>
+      </c>
+      <c r="G461" s="7" t="s">
+        <v>4802</v>
       </c>
     </row>
     <row r="462" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -36774,8 +36841,11 @@
       <c r="E478" s="1" t="s">
         <v>4771</v>
       </c>
-      <c r="G478">
+      <c r="F478" s="7">
         <v>1</v>
+      </c>
+      <c r="G478" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="479" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -36827,8 +36897,11 @@
       <c r="E482" s="1" t="s">
         <v>4773</v>
       </c>
-      <c r="G482">
+      <c r="F482" s="7">
         <v>1</v>
+      </c>
+      <c r="G482" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="483" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -37063,8 +37136,11 @@
       <c r="E501" s="1" t="s">
         <v>4776</v>
       </c>
-      <c r="G501">
+      <c r="F501" s="7">
         <v>2</v>
+      </c>
+      <c r="G501" s="7" t="s">
+        <v>4585</v>
       </c>
     </row>
     <row r="502" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37122,8 +37198,11 @@
       <c r="E505" s="1" t="s">
         <v>4639</v>
       </c>
-      <c r="G505">
+      <c r="F505" s="7">
         <v>1</v>
+      </c>
+      <c r="G505" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="506" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37153,8 +37232,11 @@
       <c r="E507" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G507">
+      <c r="F507" s="7">
         <v>1</v>
+      </c>
+      <c r="G507" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="508" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37195,8 +37277,11 @@
       <c r="E510" s="1" t="s">
         <v>4742</v>
       </c>
-      <c r="G510">
+      <c r="F510" s="7">
         <v>1</v>
+      </c>
+      <c r="G510" s="7" t="s">
+        <v>4587</v>
       </c>
     </row>
     <row r="511" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37215,8 +37300,11 @@
       <c r="E511" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G511">
+      <c r="F511" s="7">
         <v>1</v>
+      </c>
+      <c r="G511" s="7" t="s">
+        <v>4584</v>
       </c>
     </row>
     <row r="512" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37235,8 +37323,11 @@
       <c r="E512" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G512">
+      <c r="F512" s="7">
         <v>1</v>
+      </c>
+      <c r="G512" s="7" t="s">
+        <v>4578</v>
       </c>
     </row>
     <row r="513" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37343,8 +37434,11 @@
       <c r="E521" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G521">
+      <c r="F521" s="7">
         <v>2</v>
+      </c>
+      <c r="G521" s="7" t="s">
+        <v>4819</v>
       </c>
     </row>
     <row r="522" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37385,8 +37479,11 @@
       <c r="E524" s="1" t="s">
         <v>4783</v>
       </c>
-      <c r="G524">
+      <c r="F524" s="7">
         <v>1</v>
+      </c>
+      <c r="G524" s="7" t="s">
+        <v>4803</v>
       </c>
     </row>
     <row r="525" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37455,8 +37552,11 @@
       <c r="E529" s="1" t="s">
         <v>4672</v>
       </c>
-      <c r="G529">
+      <c r="F529" s="7">
         <v>1</v>
+      </c>
+      <c r="G529" s="7" t="s">
+        <v>4578</v>
       </c>
     </row>
     <row r="530" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37486,8 +37586,11 @@
       <c r="E531" s="1" t="s">
         <v>4799</v>
       </c>
-      <c r="G531" s="1">
+      <c r="F531" s="7">
         <v>1</v>
+      </c>
+      <c r="G531" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="532" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37517,8 +37620,11 @@
       <c r="E533" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G533">
+      <c r="F533" s="7">
         <v>2</v>
+      </c>
+      <c r="G533" s="7" t="s">
+        <v>4840</v>
       </c>
     </row>
     <row r="534" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37548,8 +37654,11 @@
       <c r="E535" s="1" t="s">
         <v>4786</v>
       </c>
-      <c r="G535">
+      <c r="F535" s="7">
         <v>1</v>
+      </c>
+      <c r="G535" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="536" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37579,8 +37688,11 @@
       <c r="E537" s="1" t="s">
         <v>4786</v>
       </c>
-      <c r="G537">
+      <c r="F537" s="7">
         <v>1</v>
+      </c>
+      <c r="G537" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="538" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37610,8 +37722,11 @@
       <c r="E539" s="1" t="s">
         <v>4786</v>
       </c>
-      <c r="G539">
+      <c r="F539" s="7">
         <v>1</v>
+      </c>
+      <c r="G539" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="540" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37641,8 +37756,11 @@
       <c r="E541" s="1" t="s">
         <v>4786</v>
       </c>
-      <c r="G541">
+      <c r="F541" s="7">
         <v>1</v>
+      </c>
+      <c r="G541" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="542" spans="1:7" ht="160" x14ac:dyDescent="0.2">
@@ -37661,8 +37779,11 @@
       <c r="E542" s="1" t="s">
         <v>4535</v>
       </c>
-      <c r="G542">
+      <c r="F542" s="7">
         <v>2</v>
+      </c>
+      <c r="G542" s="7" t="s">
+        <v>4588</v>
       </c>
     </row>
     <row r="543" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -37692,8 +37813,11 @@
       <c r="E544" s="1" t="s">
         <v>4639</v>
       </c>
-      <c r="G544">
+      <c r="F544" s="7">
         <v>1</v>
+      </c>
+      <c r="G544" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37712,8 +37836,11 @@
       <c r="E545" s="1" t="s">
         <v>4793</v>
       </c>
-      <c r="G545">
+      <c r="F545" s="7">
         <v>2</v>
+      </c>
+      <c r="G545" s="7" t="s">
+        <v>4805</v>
       </c>
     </row>
     <row r="546" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37732,8 +37859,11 @@
       <c r="E546" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G546">
+      <c r="F546" s="7">
         <v>1</v>
+      </c>
+      <c r="G546" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="547" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -37752,8 +37882,11 @@
       <c r="E547" s="1" t="s">
         <v>4786</v>
       </c>
-      <c r="G547">
+      <c r="F547" s="7">
         <v>2</v>
+      </c>
+      <c r="G547" s="7" t="s">
+        <v>4813</v>
       </c>
     </row>
     <row r="548" spans="1:7" ht="144" x14ac:dyDescent="0.2">
@@ -37772,8 +37905,11 @@
       <c r="E548" s="1" t="s">
         <v>4462</v>
       </c>
-      <c r="G548">
+      <c r="F548" s="7">
         <v>1</v>
+      </c>
+      <c r="G548" s="7" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="549" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -37792,8 +37928,11 @@
       <c r="E549" s="1" t="s">
         <v>4497</v>
       </c>
-      <c r="G549">
+      <c r="F549" s="7">
         <v>1</v>
+      </c>
+      <c r="G549" s="7" t="s">
+        <v>4583</v>
       </c>
     </row>
     <row r="550" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -38599,8 +38738,11 @@
       <c r="E621" s="1" t="s">
         <v>4827</v>
       </c>
-      <c r="G621">
+      <c r="F621" s="7">
         <v>4</v>
+      </c>
+      <c r="G621" s="1" t="s">
+        <v>4841</v>
       </c>
     </row>
     <row r="622" spans="1:7" ht="96" x14ac:dyDescent="0.2">

</xml_diff>